<commit_message>
Adding work by Miika Lehtinen.
</commit_message>
<xml_diff>
--- a/src/morphology/incoming/Compg_sms.xlsx
+++ b/src/morphology/incoming/Compg_sms.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6898" uniqueCount="3950">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7888" uniqueCount="4494">
   <si>
     <t xml:space="preserve">Tyyppi</t>
   </si>
@@ -12041,6 +12041,1638 @@
   </si>
   <si>
     <t xml:space="preserve">VJO s. 77</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12.5.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aaunâsmuõrid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aaunâsmuõrr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tarvepuu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aaunâs+muõrr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aine+puu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tõiʹnn pieʹʒʒin raʹjje aaunâsmuõrid: nueʹttoolǥid, säiʹmmoolǥid, võõnâsteälaid, moostid, kaartid da nuʹtt ooudâs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Niistä männyistä tehtiin tarvepuuta: nuottaulkuja, verkkoulkuja, veneen teloja, siltoja, kaukaloita ja niin edelleen. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VJO s. 75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arggporrmõõžž</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arggporrmõš</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arkiruoka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">argg+porrmõš</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arki+ruoka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tõk leʹjje tuâlʼja vuäʹmm saaʹmi arggporrmõõžž.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ne olivat ennen vanhaan vanhoja kolttien arkiruokia. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ceäggmuõrid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ceäggmuõrr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pystyssä oleva puu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ceägg+muõrr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pysty+puu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nâ seämmanalla ǩeʹldde, što ceäggmuõrid iǥõl vueʹtǩǩed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No samalla tavalla kielsivät, ettei pystyssä olevia puita saa kuloa. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">čeäpstõk-kuurta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">naisen pusero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">čeäpstõk+kuurta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tamppi (vyömäinen kangaskaistale)+naisen pusero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toʹben puʹhtte muʹnne säiʹmmčâʹlmmgaaʹrestkååut da čeäpstõk-kuurta.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sieltä toivat minulle verkkokangashameen ja puseron. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">čuäʹrvvkåållmin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">čuäʹrvvkåållam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sarvikuloin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">čuäʹrvv+kåållam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sarvi+kuloin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">De čuäʹrvvkåållmin kålla de räʹjje da koškkâd peʹjje de ellsest iŋŋee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sitten kulovat sarvikuloimella ja valmistavat ja panevat kuivumaan ja kuivattavat hiilloksessa. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">čääʹcctuõʹllʼjeei</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vedenpitävä</t>
+  </si>
+  <si>
+    <t xml:space="preserve">čääʹcc+tuõʹllʼjeei</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vesi+pitävä</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tõk liâ čääʹcctuõʹllʼjeei pihttâz, što nueʹttmen ij kaast.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ne ovat vedenpitävät vaatteet, ettei kastu nuotatessa. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VJO s. 76</t>
+  </si>
+  <si>
+    <t xml:space="preserve">heäʹrvvkååutid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">heäʹrvvkåhtt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">koristeellinen hame</t>
+  </si>
+  <si>
+    <t xml:space="preserve">heäʹrvv+kåhtt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">koriste+hame</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tõiʹd Taarâst puʹhtte, tõiʹnn eʹpet heäʹrvvkååutid raajât.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Niitä toivat Norjasta, niistä taas tehdään koristeellisia hameita. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">juõʹǩǩpeivvsaž</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jokapäiväinen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">juõʹǩǩ+peivvsaž</t>
+  </si>
+  <si>
+    <t xml:space="preserve">joka+päiväinen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adv+A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">juõʹǩǩpeivvsaž jieʹllem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jokapäiväinen elämä</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jälstemsââi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jälstemsââʹjj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jälstem+sââʹjj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asuminen+paikka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ǩeäʹstt-a mâʹmmet liâ jälstemsââi, koozz jäämm, de tõzz-i rueʹǩǩe.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kenellä on minkäkin verran asuinpaikkoja, mihin kuolee, niin siihen hautaavat. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VJO s. 79</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kauppkueʹllšeeʹllemäiʹǧǧ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">myytävän kalan pyyntiaika</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kauppkueʹll+šeeʹllemäiʹǧǧ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kauppakala+pyydystysaika</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N(nom)N(Nom)+V(akt)N(Nom)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Čõhčč šâdd de tõt kauppkueʹllšeeʹllemäiʹǧǧ poott.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Syksy tulee ja myytävän kalan pyyntiaika loppuu. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ǩeʹttemǩieʹmn </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ǩeʹttemǩieʹmnn </t>
+  </si>
+  <si>
+    <t xml:space="preserve">keittokattila</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ǩeʹttem+ǩieʹmnn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">keittäminen+kattila</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Måtmin iʹlla ni mii, di ǩeʹttemǩieʹmn väʹldde.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joillakuilla ei ole mitään, niin ottavat keittokattilan. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">koomačkåhtt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">damastihame</t>
+  </si>
+  <si>
+    <t xml:space="preserve">koomač+kåhtt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">damasti(?)+hame</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Šõõddi mâʹta ruõʹpsses koomačkåhtt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Siitä] tuli kuin punainen damastihame.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kueʹllšiiʹli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kueʹllšiiʹlli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kalastaja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kueʹll+šiiʹlli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kala+pyydystäjä</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tuållâmsiidâst puk leʹjje kueʹllšiiʹli.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tuuloman kylässä kaikki olivat kalastajia. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kueʹllvuõjj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kalanrasva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kueʹll+vuõjj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kala+voi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">De kueʹllvuõjj ku lij, porškuäʹtte de tõn peejj tõõzz vuâlla mâʹta huutt diǥu.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kun on kalanrasvaa, rupeavat syömään ja sitä (pettua) panevat siihen alle, niin kuin puuroa. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kueʹttkõõsk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kueʹttkõskk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kotien väli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kueʹtt+kõskk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kota+väli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nuʹtt liâ kuuʹǩǩ kueʹttkõõsk, måtmin kueʹttkõõskin kollai piânnai uukkâm, jäänaš ij kullu.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kotien välit ovat niin pitkät, joillakin väleillä kuuluu koiran haukunta, enimmäkseen ei kuulu. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kuuđnieʹttlõõzzâž</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kuusiviikkoinen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kuuđ+nieʹttlõõzzâž</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kuusi+viikkoinen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Num(gen)+A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Piârân leäi õhtt nijdd, tõt leäi kuuđnieʹttlõõzzâž, teä jaaʹmi.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perheenä oli yksi tytär, se oli kuusiviikkoinen, sitten kuoli. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">leiʹbbtäiʹǧǧ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">leipätaikina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">leiʹbb+täiʹǧǧ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">leipä+taikina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Veärrliõm kuäivai de tõiʹnn soʹtǩǩii, tõʹst šõõddi mâʹta leiʹbbtäiʹǧǧ diǥu.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kauhaisi keittolientä ja sekoitti sen kanssa, siitä tuli kuin leipätaikinaa. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">leäʹppčääʹʒʒest </t>
+  </si>
+  <si>
+    <t xml:space="preserve">leäʹppčääʹcc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">leppäparkkiliemi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">leäʹpp+čääʹcc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">leppä+vesi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mon vaʹlddem pâi lieʹppid viǯǯlem de leäʹppčääʹʒʒest tuõlddeem tõn kåhttan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minä hain vain lepän kuoria (sananmukaisesti: leppiä) ja keitin sen hameeni leppäparkkiliemessä. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">luõssjokk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lohijoki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">luõss+jokk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lohi+joki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nåkam leäi luõssjokk tõt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sellainen lohijoki se oli. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">lääʹddǩiõll</t>
+  </si>
+  <si>
+    <t xml:space="preserve">suomen kieli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lääʹdd+ǩiõll</t>
+  </si>
+  <si>
+    <t xml:space="preserve">suomi+kieli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kâʹl lääʹddǩiõll ij jååttam.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kyllä suomen kieli ei luistanut. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">meäʹccjieʹllem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">elämä luonnossa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meäʹcc+jieʹllem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">metsä+elämä</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tõt leäi jeeʹres jieʹllem saaʹmin, meäʹccjieʹllem leäi.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Koltilla oli erilainen elämä, se oli elämää luonnossa. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">muõrrmaddjest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">muõrrmaadd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">puun tyvi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">muõrr+maadd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">puu+tyvi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vuõššân âlgg väʹldded kõõr muõrrmaddjest vueʹtǩǩmin.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ensin täytyy ottaa kuori puun tyvestä kuloimella. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">mättʼtõsäiʹǧǧ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">opetusaika</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mättʼtõs+äiʹǧǧ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">opetus+aika</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kuäʹss päärnain ku lij mättʼtõsäiʹǧǧ, toʹb tueʹǩǩen liâ kavvâz, pâi zääʹvesǩ ouʹdde roʹttješ.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kun lapsilla on opetusaika, siellä takana on ikoneita, vain verho vedettiin väliin. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">nelljloekksaž</t>
+  </si>
+  <si>
+    <t xml:space="preserve">neljäkymmentävuotias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nelljlo+ekksaž</t>
+  </si>
+  <si>
+    <t xml:space="preserve">neljäkymmentä+vuotinen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nuʹtt te leʹjjem, håʹt leʹjjem 40-ekksaž, pâʹjjel.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Niin olin, vaikka olin neljäkymmentävuotias, ylikin.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">njââʹllvaaldõõzz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">njââʹllvaaldõs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jälsikerros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">njââʹll+vaaldõs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nila+?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">De veʹǩǩe põrttseez de kõõrâst tõn viõʹlǧǧes njââʹllvaaldõõzz väʹldde.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sitten vievät kotiinsa ja ottavat kuoresta sen valkoisen jälsikerroksen. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">njââʹlläiʹǧǧ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nila-aika</t>
+  </si>
+  <si>
+    <t xml:space="preserve">njââʹll+äiʹǧǧ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nila+aika</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pieʹʒʒid âʹte ǥu raajât, âlgg leeʹd njââʹlläiʹǧǧ.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kun tehdään pettua, pitää olla nila-aika. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">nueʹttempihttâz </t>
+  </si>
+  <si>
+    <t xml:space="preserve">nueʹttempiiutâs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nuottausvaate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nueʹttem+piiutâs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nuottaaminen+vaate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nueʹttempihttâz leʹjje.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nuottausvaatteet olivat. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">nueʹttoolǥid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nueʹttolgg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nuottaulku (salko)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nueʹtt+olgg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nuotta+ulklu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">piiđvaaʹldi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">piiđvaʹlddi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">veronkantaja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">piiđ+vaʹlddi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vero+ottaja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N(nom/gen(?)+N(agnt)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Piiđvaaʹldi seeʹst ǩieʹmn väʹldde, määccaǩ lij âʹlnn de tõn jäʹhsse piiđâst.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Veronkantajat ottivat heiltä kattilan, takki on päällä ja senkin riisuvat veroksi. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">puäʹrespeiʹvv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vanhuuden päivät (?)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">puäʹres+peiʹvv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vanha+päivä</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A(attr/pred)+N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Äiʹǧǧ lij nuʹtt pijjum. Ǩeäzz ââʹǩǩ lij puäʹrespeiʹvv.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aika on niin asetettu. (Sananmukainen käännös lopusta: Kenelle aika on vanha-päivä. Tarkoittaa ehkä: Kuka nyt vanhaksi elääkin. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ruõkkâmpoodd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ruõkkâmpodd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hautaushetki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ruõkkâm+podd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hautaaminen+hetki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kook pihttsid räʹjje da pâʹsse da maddu peʹjje, teʹl pâi tõk puõʹtte ruõkkâmpoodd.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jotka tekevät vaatteet ja pesevät ja maahan panevat, silloin vain ne tulevat hautaushetkellä. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ruõššǩeeʹrj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ruõššǩeʹrjj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">venäläinen kirjain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ruõšš+ǩeʹrjj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">venäjä+kirjain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Âʹlǧǧe leeʹd nåkam ååʹšǩ lookkâd ruõššǩeeʹrj.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pitää olla sellaiset silmälasit venäläisten kirjainten lukemiseen. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ruõššääiʹjest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ruõššäiʹǧǧ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Venäjän aika</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ruõšš+äiʹǧǧ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Venäjä+aika</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toʹben leäi ruõššääiʹjest luõvâs meäʹcc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Siellä oli Venäjän aikaan vapaata metsää. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sijddpääiʹǩest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sijddpäiʹǩǩ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kyläpaikka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sijdd+päiʹǩǩ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kylä+paikka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nâ tän sijddpääiʹǩest mõõk liâ kuõʹlid.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No mitäpä kaloja täällä kyläpaikassa on. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">suäjjkååutid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">suäjjkåhtt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hihallinen hame (=mekko?)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">suäjj+kåhtt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hiha+hame</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kook leʹjje reggsab oummu, tõk vuäʹstte värjjaunnsid de tõiʹnn neezzan suäjjkååutid kuårru mâʹta määccǩid diǥu.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jotka olivat rikkaampia ihmisiä, ne ostivat loudekankaita ja niistä naiset ompelivat hihallisia hameita (=mekkoja?), niin kuin takkeja. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">säiʹmmoolǥid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">säiʹmm+olgg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verkkoulku</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verkko+ulku</t>
+  </si>
+  <si>
+    <t xml:space="preserve">säiʹmmčâʹlmmgaaʹrestkååut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">säiʹmmčâʹlmmgaaʹrestkåhtt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verkkokangashame</t>
+  </si>
+  <si>
+    <t xml:space="preserve">säiʹmmčâʹlmmgaarest+kåhtt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verkkosilmäkangas+hame</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tiuddvuäzzlaž</t>
+  </si>
+  <si>
+    <t xml:space="preserve">täyden osan saava</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tiudd+vuäzzlaž</t>
+  </si>
+  <si>
+    <t xml:space="preserve">täysi+osallinen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A(attr)+A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leâša teʹl leäi nijdd vueʹsspieʹllooumaž, åålmpäʹrnn leäi tiuddvuäzzlaž.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mutta silloin tytölle tuli vain puoli osaa (sananmukaisesti: tyttö oli puoliosaihminen), poikalapsi sai täyden osan (sananmukaisesti: oli täysiosallinen). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tuållâmjokkšeeʹllem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tuulomanjoen kalastus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tuållâmjokk+šeeʹllem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tuulomanjoki+kalastus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N(nom)+N(V(akt))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ku Tuâllamjokkšeeʹllem peällʼlõõžži, teʹl Tuâllamjokk puk kaaʹtti tõiʹd piiđid.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Siihen aikaan] kun [meillä oli] Tuulomanjoen kalastus puoliksi, silloin Tuulomanjoki kattoi kaikki ne verot. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">veärrliõm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">veärrliõmm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">keittoliemi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">veärr+liõmm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">keitto+liemi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">võõnâsteälaid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">võõnâsteälaž</t>
+  </si>
+  <si>
+    <t xml:space="preserve">veneentela</t>
+  </si>
+  <si>
+    <t xml:space="preserve">võõnâs+teälaž</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vene+tela</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vueʹsspieʹll</t>
+  </si>
+  <si>
+    <t xml:space="preserve">puolikas osa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vueʹss+pieʹll</t>
+  </si>
+  <si>
+    <t xml:space="preserve">osa+puoli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A ââʹn Lääʹddest liâ kuhttu õõutnalla, åålmai da neezzan, ij ni kuäbbaž vueʹsspieʹll.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ja nyt Suomessa molemmat ovat samalla tavalla, mies ja nainen, ei kumpikaan puoliosainen (sananmukaisesti: osapuoli).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vueʹsspieʹllooumaž</t>
+  </si>
+  <si>
+    <t xml:space="preserve">puolikkaan osan saava</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vueʹsspieʹll+ooumaž</t>
+  </si>
+  <si>
+    <t xml:space="preserve">osapuoli+ihminen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N(nom)N(Nom)+N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vueʹtǩǩempieʹccen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vueʹtǩǩempieʹcc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kulottava mänty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vueʹtǩǩem+pieʹcc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kulominen+mänty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tõʹnt vueʹtǩǩempieʹccen vaʹlljee šõʹlles pieʹʒʒid.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Siksi kulottavaksi valittiin sileitä mäntyjä. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">värjjaunnsid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">värjjaaunâs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">loudekangas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">värjj+aaunâs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">loude+aine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">årstõk-kååutas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">årstõk-kåhtt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">säkkikangashame</t>
+  </si>
+  <si>
+    <t xml:space="preserve">årstõk+kåhtt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">säkkikangas+hame</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Årstõk-kååutas pääinai lieʹppin.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Säkkikangashameensa värjäsi lepällä. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">åålmpäʹrnn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">poikalapsi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">åålm+päʹrnn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mies+lapsi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ââʹzzteeʹm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ââʹzzteʹm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ohut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ââʹss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kesi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N &gt; A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A faaʹnal leʹjje ââʹzzteeʹm, a gallmaant, tõk liâ âssai da ravvsab.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flanellit olivat ohuita ja galmantit (?), ne olivat paksuja ja vahvempia. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">âlddlõõžži</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lähekkäin </t>
+  </si>
+  <si>
+    <t xml:space="preserve">âʹldd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lähi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N &gt; Adv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tõk juʹn liâ âlddlõõžži, ǥo pieʹnne jiõnn kollai.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ne ovat jo lähekkäin, jos koiran ääni kuuluu. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">âssai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">paksu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">huõllâm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">huõllâd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">huolia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">huõll</t>
+  </si>
+  <si>
+    <t xml:space="preserve">huoli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N &gt; V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eiʹdde tâma kâʹl tättad leʹjjem, jiõččan nõõm leʹjjem ǩeeʹrjted, leâša jiõm huõllâm.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tahtonut kyllä olisin, olisin kirjoittanut oman nimeni, mutta en huolinut. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">iŋŋee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iŋŋeed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kuivattaa (rutikuivaksi)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iiŋâs # iŋŋ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rutikuiva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A &gt; V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jaaʹmi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V &gt; N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tõʹst ââlda vuäʹmm jaaʹmi ku liâ, teʹl veʹǩǩe õõut­sâjja.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jos siinä lähellä on vanhoja vainajia, niin vievät samaan pakkaan. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">jiijjâznallšem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">omanlaisensa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jiõčč</t>
+  </si>
+  <si>
+    <t xml:space="preserve">itse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pron(Px3Pl) &gt; Adv </t>
+  </si>
+  <si>
+    <t xml:space="preserve">nallšem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pâi jiijj kuärra jiijjâznallšem pihttsid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Itse vain ompelevat omanlaisiaan vaatteita. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">jiõnnsa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ääneen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jiõnn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ääni</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teʹl leäi, jiõnnsa reäǥǥeeʹl pråʹššjõʹtte.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silloin oli, ääneen itkien jättivät hyvästit. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">jäävvteeʹm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jäävvteʹm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jauhoton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jävv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jauho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A jäävv ku leʹjje occanj, kook jäävvteeʹm leʹjje, de tõk leeiʹb sâjja tõn raʹjje.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kun jauhoja oli vähän, [ne] joilla ei ollut jauhoja (sananmukaisesti: olivat jauhottomia), tekivät sitä (pettupuuroa) leivän sijaan.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ǩeeʹrjteʹmes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ǩeeʹrjteʹm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lukutaidoton (sananmukaisesti: kirjaton)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mij leeiʹm ǩeeʹrjteʹmes oummu.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Me olimme lukutaidottomia (sananmukaisesti: kirjattomia) ihmisiä. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kuärstem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V &gt; V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A mon kååut kuärstem, tõn suäjjkååut.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ja minä ompelin hameen, sen hihallisen hameen (=mekon?).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(čuäʹrvv)kåållmin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kåållam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kuloin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kåållad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kuloa (irrottaa männyn kuorta)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tõn tiõʹđi ku peiʹvv pirr ââʹlm jåått da piõgg muõrid da čääʹʒʒ liikktââll.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sen tiesi kun aurinko kulkee pitkin taivasta ja tuuli liikuttelee puita ja vettä. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">moʹttai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moʹttjed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">murskata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*mååttad / måttad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">De norddmõõzzin moʹttai tõn tueʹllj leʹbe mõõn-ne âʹlnn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sitten murskaa petkeleellä taljan tai jonkin sellaisen päällä. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vrt. Mottned ‹murskautua› </t>
+  </si>
+  <si>
+    <t xml:space="preserve">mättʼtõs(äiʹǧǧ)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mättʼtõs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">opetus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mättʼted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mäŋggsest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">määŋgas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moni ihminen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mäŋgg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moni</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Num &gt; N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mon leäm mäŋggsest kuâđđjam.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Olen menettänyt monta läheistäni (sananmukaisesti: Olen jäänyt monesta.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(kuuđ)nieʹttlõõzzâž</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nieʹttlõõzzâž</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-viikkoinen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nieʹttel </t>
+  </si>
+  <si>
+    <t xml:space="preserve">viikko</t>
+  </si>
+  <si>
+    <t xml:space="preserve">õõzzâž</t>
+  </si>
+  <si>
+    <t xml:space="preserve">norddmõõzzin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">norddmõs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pettupetkel, survoin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">norddâd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">survoa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mõs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ǩirggan de čuäckk, pâi norddmõõzzin nordškuätt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kun [pettu] valmistuu ja viilenee, rupeaa survomaan petkeleellä.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nårrai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nårrjed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kerääntyä, kertyä</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mäʹhssed ij vueiʹt, nårrai nårrai, ǩeäinn liâ põõrt, ǩeäinn mõõk leʹžže, puk mâʹnne.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ei voi maksaa, [vero] kerääntyy [ja] kerääntyy, kenellä on talo ja keillä mitä lieneekään, kaikki menevät. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">occanj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vähän</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A &gt; Adv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">anj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jävv nuʹtt ij peeʹšt kuuʹǩǩ ku occanj lij.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jauho ei kestä pitkään, kun [sitä] on vähän. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(juõʹǩǩ)peivvsaž</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-peivvsaž</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-päiväinen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">peiʹvv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">päivä</t>
+  </si>
+  <si>
+    <t xml:space="preserve">peällʼlõõžži</t>
+  </si>
+  <si>
+    <t xml:space="preserve">puoliksi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pieʹll</t>
+  </si>
+  <si>
+    <t xml:space="preserve">puoli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kaaupše kuõʹlid di tieʹǧǧid puk juõʹǩǩe peällʼlõõžži.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Möivät kalat ja panivat kaikki rahat puoliksi.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">põõlâč</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pelokas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V &gt; A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mon leʹjjem nuʹtt põõlâč, da nuʹtt-i leʹjje še måtam, põõlee.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minä olin niin pelokas, ja niin olivat jotkut [muut]kin, pelkäsivät. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">põõlee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">põõleed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pelätä (kont.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">poorti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tuållâmjokk tõt leäi: poorti da piiđid maauʹsi.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tuulomajoki se oli: ruokki (sananmukaisesti: syötti) ja maksoi verot. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">pråʹššjõʹtte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pråʹššjõõttâd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jättää hyvästit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*pråʹššjed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">puäʹresvuõtt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vanhuus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">puäʹres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A &gt; N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vuõtt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Puäʹresvuõtt tõn âma ceäʹlǩǩe, što tõt iʹlla räädast.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vanhuus, siitähän sanotaan, ettei se ole ilo. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rõsseed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">puuhailla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*rõõssâd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mõõn vuõiʹti da mõõn ǩirggni rõsseed, tõn-i tuejjii.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mitä pystyi ja mitä ehti puuhaamaan, sen teki. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ruõššâs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">venäjäksi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ruõšš</t>
+  </si>
+  <si>
+    <t xml:space="preserve">venäjä</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ruõššâs kâʹl siltteem, leâša ââʹn leäm puk väjldâttam.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Venäjäksi kyllä osasin [puhua], mutta nyt olen unohtanut kaiken. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">saaʹminallšem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kolttien tapainen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ânnʼjõž ääiʹjest sääʹmjieʹllem iʹlla ni vooʹps tuâlʼjõž saaʹminallšem jieʹllem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nykyaikana kolttien elämä ei ole lainkaan entistä kolttien tapaista elämää. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Tuâllamjokk)šeeʹllem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">šeeʹllem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pyydystäminen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">šeeʹlled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pyydystää</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sieʹjjat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sieʹjjted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sekoittaa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sieʹǩǩ- </t>
+  </si>
+  <si>
+    <t xml:space="preserve">seka-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">De tõn mâŋŋa jäävvaivuiʹm sieʹjjat de veär ǩeâtt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sen jälkeen sekoittaa jauhojen kanssa ja keittää keittoa. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vrt. seäkkned ‹sekaantua› </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(kueʹll)šiiʹli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">šiiʹlli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pyydystäjä</t>
+  </si>
+  <si>
+    <t xml:space="preserve">šõddi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kasvava</t>
+  </si>
+  <si>
+    <t xml:space="preserve">šõddâd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kasvaa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">De mon mošttjem, ǥo leʹjjem šõddi niõđâž, eʹčč da jeäʹnn jiõʹlle Peäccmest.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sähss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sähssad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">likaantua</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lika</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mäʹhtt mon vuäitam nueʹtted, sähss čuuʹt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Miten voin nuotata, [hame] likaantuu kovin. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">säämas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">koltansaameksi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">as</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Måttam jõõll liâ nuʹtt što säämas iǥõl särnnad, ašttõʹlle.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jotkut hupsut sanovat, ettei koltansaameksi pidä puhua, kerrotaan. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(võõnâs)teälaid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">teälaž</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tela (dem.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tieʹll</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tela</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N &gt; N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tuõlddeem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tuõlddeed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">keittää</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(čääʹcc)tuõʹllʼjeei</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tuõʹllʼjeei</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pitävä</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tuõʹllʼjed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(piiđ)vaaʹldi </t>
+  </si>
+  <si>
+    <t xml:space="preserve">vaʹlddi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ottaja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">veänccõõttâm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">veänccõõttâd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">veäncceed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vihkiä</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Papp kuäʹss puätt põõʹzzid leʹbe veänccõõttâm diõtt kåčča, de škooulâst-i õʹnne.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kun pappi tulee pyhinä tai kutsutaan häiden takia, [tilaisuus] pidettiin koulussa. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">viirtet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vueʹtǩǩmin pirr vääʹldet de mâŋŋa pieʹʒʒ viirtet.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kuloimella otetaan ympäri ja sitten kaadetaan mänty. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">virsseed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">laulaa itkuvirsiä</t>
+  </si>
+  <si>
+    <t xml:space="preserve">virss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">itkuvirsi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silttääm mon kâʹl virsseed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Osaan kyllä laulaa itkuvirsiä. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">viǯǯlem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vueʹtǩǩmin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vueʹtǩǩem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vueʹtǩǩed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(tiudd)vuäzzlaž</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vuäzzlaž</t>
+  </si>
+  <si>
+    <t xml:space="preserve">osallinen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">osa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">väjldââʹtt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*väjlded</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V &gt; V (?)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mon âʹte jiõm väjldââʹtt ouddâl tõn pääiʹǩ ǥu tunâlmma mõõnžem.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minä en unohda sitä paikkaa ennen kuin menen tuonpuoleiseen. </t>
   </si>
 </sst>
 </file>
@@ -12206,25 +13838,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L666"/>
+  <dimension ref="A1:L762"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G609" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I622" activeCellId="0" sqref="I622"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A665" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A668" activeCellId="0" sqref="A668"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="32.2908163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.6428571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.1530612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.3316326530612"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.8775510204082"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.234693877551"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.8928571428571"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.6224489795918"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.3469387755102"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="16.2551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="10.3469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="34.5561224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.6989795918367"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.9591836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.6887755102041"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.5765306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.2551020408163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="26.6020408163265"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.219387755102"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17.280612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34219,6 +35849,3166 @@
       </c>
       <c r="K666" s="0" t="s">
         <v>3949</v>
+      </c>
+    </row>
+    <row r="668" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B668" s="3" t="s">
+        <v>3950</v>
+      </c>
+    </row>
+    <row r="669" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A669" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B669" s="0" t="s">
+        <v>3951</v>
+      </c>
+      <c r="C669" s="0" t="s">
+        <v>3952</v>
+      </c>
+      <c r="D669" s="0" t="s">
+        <v>3953</v>
+      </c>
+      <c r="E669" s="0" t="s">
+        <v>3954</v>
+      </c>
+      <c r="F669" s="0" t="s">
+        <v>3955</v>
+      </c>
+      <c r="G669" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I669" s="0" t="s">
+        <v>3956</v>
+      </c>
+      <c r="J669" s="0" t="s">
+        <v>3957</v>
+      </c>
+      <c r="K669" s="0" t="s">
+        <v>3958</v>
+      </c>
+    </row>
+    <row r="670" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A670" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B670" s="0" t="s">
+        <v>3959</v>
+      </c>
+      <c r="C670" s="0" t="s">
+        <v>3960</v>
+      </c>
+      <c r="D670" s="0" t="s">
+        <v>3961</v>
+      </c>
+      <c r="E670" s="0" t="s">
+        <v>3962</v>
+      </c>
+      <c r="F670" s="0" t="s">
+        <v>3963</v>
+      </c>
+      <c r="G670" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I670" s="0" t="s">
+        <v>3964</v>
+      </c>
+      <c r="J670" s="0" t="s">
+        <v>3965</v>
+      </c>
+      <c r="K670" s="0" t="s">
+        <v>3489</v>
+      </c>
+    </row>
+    <row r="671" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A671" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B671" s="0" t="s">
+        <v>3966</v>
+      </c>
+      <c r="C671" s="0" t="s">
+        <v>3967</v>
+      </c>
+      <c r="D671" s="0" t="s">
+        <v>3968</v>
+      </c>
+      <c r="E671" s="0" t="s">
+        <v>3969</v>
+      </c>
+      <c r="F671" s="0" t="s">
+        <v>3970</v>
+      </c>
+      <c r="G671" s="0" t="s">
+        <v>1087</v>
+      </c>
+      <c r="I671" s="0" t="s">
+        <v>3971</v>
+      </c>
+      <c r="J671" s="0" t="s">
+        <v>3972</v>
+      </c>
+      <c r="K671" s="0" t="s">
+        <v>3958</v>
+      </c>
+    </row>
+    <row r="672" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A672" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B672" s="0" t="s">
+        <v>3973</v>
+      </c>
+      <c r="C672" s="0" t="s">
+        <v>3973</v>
+      </c>
+      <c r="D672" s="0" t="s">
+        <v>3974</v>
+      </c>
+      <c r="E672" s="0" t="s">
+        <v>3975</v>
+      </c>
+      <c r="F672" s="0" t="s">
+        <v>3976</v>
+      </c>
+      <c r="G672" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I672" s="0" t="s">
+        <v>3977</v>
+      </c>
+      <c r="J672" s="0" t="s">
+        <v>3978</v>
+      </c>
+      <c r="K672" s="0" t="s">
+        <v>3958</v>
+      </c>
+    </row>
+    <row r="673" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A673" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B673" s="0" t="s">
+        <v>3979</v>
+      </c>
+      <c r="C673" s="0" t="s">
+        <v>3980</v>
+      </c>
+      <c r="D673" s="0" t="s">
+        <v>3981</v>
+      </c>
+      <c r="E673" s="0" t="s">
+        <v>3982</v>
+      </c>
+      <c r="F673" s="0" t="s">
+        <v>3983</v>
+      </c>
+      <c r="G673" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I673" s="0" t="s">
+        <v>3984</v>
+      </c>
+      <c r="J673" s="0" t="s">
+        <v>3985</v>
+      </c>
+      <c r="K673" s="0" t="s">
+        <v>3489</v>
+      </c>
+    </row>
+    <row r="674" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A674" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B674" s="0" t="s">
+        <v>3986</v>
+      </c>
+      <c r="C674" s="0" t="s">
+        <v>3986</v>
+      </c>
+      <c r="D674" s="0" t="s">
+        <v>3987</v>
+      </c>
+      <c r="E674" s="0" t="s">
+        <v>3988</v>
+      </c>
+      <c r="F674" s="0" t="s">
+        <v>3989</v>
+      </c>
+      <c r="G674" s="0" t="s">
+        <v>2461</v>
+      </c>
+      <c r="I674" s="0" t="s">
+        <v>3990</v>
+      </c>
+      <c r="J674" s="0" t="s">
+        <v>3991</v>
+      </c>
+      <c r="K674" s="0" t="s">
+        <v>3992</v>
+      </c>
+    </row>
+    <row r="675" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A675" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B675" s="0" t="s">
+        <v>3993</v>
+      </c>
+      <c r="C675" s="0" t="s">
+        <v>3994</v>
+      </c>
+      <c r="D675" s="0" t="s">
+        <v>3995</v>
+      </c>
+      <c r="E675" s="0" t="s">
+        <v>3996</v>
+      </c>
+      <c r="F675" s="0" t="s">
+        <v>3997</v>
+      </c>
+      <c r="G675" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I675" s="0" t="s">
+        <v>3998</v>
+      </c>
+      <c r="J675" s="0" t="s">
+        <v>3999</v>
+      </c>
+      <c r="K675" s="0" t="s">
+        <v>3992</v>
+      </c>
+    </row>
+    <row r="676" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A676" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B676" s="0" t="s">
+        <v>4000</v>
+      </c>
+      <c r="C676" s="0" t="s">
+        <v>4000</v>
+      </c>
+      <c r="D676" s="0" t="s">
+        <v>4001</v>
+      </c>
+      <c r="E676" s="0" t="s">
+        <v>4002</v>
+      </c>
+      <c r="F676" s="0" t="s">
+        <v>4003</v>
+      </c>
+      <c r="G676" s="0" t="s">
+        <v>4004</v>
+      </c>
+      <c r="I676" s="0" t="s">
+        <v>4005</v>
+      </c>
+      <c r="J676" s="0" t="s">
+        <v>4006</v>
+      </c>
+      <c r="K676" s="0" t="s">
+        <v>3949</v>
+      </c>
+    </row>
+    <row r="677" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A677" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B677" s="0" t="s">
+        <v>4007</v>
+      </c>
+      <c r="C677" s="0" t="s">
+        <v>4008</v>
+      </c>
+      <c r="D677" s="0" t="s">
+        <v>3491</v>
+      </c>
+      <c r="E677" s="0" t="s">
+        <v>4009</v>
+      </c>
+      <c r="F677" s="0" t="s">
+        <v>4010</v>
+      </c>
+      <c r="G677" s="0" t="s">
+        <v>418</v>
+      </c>
+      <c r="I677" s="0" t="s">
+        <v>4011</v>
+      </c>
+      <c r="J677" s="0" t="s">
+        <v>4012</v>
+      </c>
+      <c r="K677" s="0" t="s">
+        <v>4013</v>
+      </c>
+    </row>
+    <row r="678" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A678" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B678" s="0" t="s">
+        <v>4014</v>
+      </c>
+      <c r="C678" s="0" t="s">
+        <v>4014</v>
+      </c>
+      <c r="D678" s="0" t="s">
+        <v>4015</v>
+      </c>
+      <c r="E678" s="0" t="s">
+        <v>4016</v>
+      </c>
+      <c r="F678" s="0" t="s">
+        <v>4017</v>
+      </c>
+      <c r="G678" s="0" t="s">
+        <v>4018</v>
+      </c>
+      <c r="I678" s="0" t="s">
+        <v>4019</v>
+      </c>
+      <c r="J678" s="0" t="s">
+        <v>4020</v>
+      </c>
+      <c r="K678" s="0" t="s">
+        <v>3992</v>
+      </c>
+    </row>
+    <row r="679" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A679" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B679" s="0" t="s">
+        <v>4021</v>
+      </c>
+      <c r="C679" s="0" t="s">
+        <v>4022</v>
+      </c>
+      <c r="D679" s="0" t="s">
+        <v>4023</v>
+      </c>
+      <c r="E679" s="0" t="s">
+        <v>4024</v>
+      </c>
+      <c r="F679" s="0" t="s">
+        <v>4025</v>
+      </c>
+      <c r="G679" s="0" t="s">
+        <v>418</v>
+      </c>
+      <c r="I679" s="0" t="s">
+        <v>4026</v>
+      </c>
+      <c r="J679" s="0" t="s">
+        <v>4027</v>
+      </c>
+      <c r="K679" s="0" t="s">
+        <v>3949</v>
+      </c>
+    </row>
+    <row r="680" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A680" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B680" s="0" t="s">
+        <v>4028</v>
+      </c>
+      <c r="C680" s="0" t="s">
+        <v>4028</v>
+      </c>
+      <c r="D680" s="0" t="s">
+        <v>4029</v>
+      </c>
+      <c r="E680" s="0" t="s">
+        <v>4030</v>
+      </c>
+      <c r="F680" s="0" t="s">
+        <v>4031</v>
+      </c>
+      <c r="G680" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I680" s="0" t="s">
+        <v>4032</v>
+      </c>
+      <c r="J680" s="0" t="s">
+        <v>4033</v>
+      </c>
+      <c r="K680" s="0" t="s">
+        <v>3992</v>
+      </c>
+    </row>
+    <row r="681" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A681" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B681" s="0" t="s">
+        <v>4034</v>
+      </c>
+      <c r="C681" s="0" t="s">
+        <v>4035</v>
+      </c>
+      <c r="D681" s="0" t="s">
+        <v>4036</v>
+      </c>
+      <c r="E681" s="0" t="s">
+        <v>4037</v>
+      </c>
+      <c r="F681" s="0" t="s">
+        <v>4038</v>
+      </c>
+      <c r="G681" s="0" t="s">
+        <v>2461</v>
+      </c>
+      <c r="I681" s="0" t="s">
+        <v>4039</v>
+      </c>
+      <c r="J681" s="0" t="s">
+        <v>4040</v>
+      </c>
+      <c r="K681" s="0" t="s">
+        <v>3992</v>
+      </c>
+    </row>
+    <row r="682" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A682" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B682" s="0" t="s">
+        <v>4041</v>
+      </c>
+      <c r="C682" s="0" t="s">
+        <v>4041</v>
+      </c>
+      <c r="D682" s="0" t="s">
+        <v>4042</v>
+      </c>
+      <c r="E682" s="0" t="s">
+        <v>4043</v>
+      </c>
+      <c r="F682" s="0" t="s">
+        <v>4044</v>
+      </c>
+      <c r="G682" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I682" s="0" t="s">
+        <v>4045</v>
+      </c>
+      <c r="J682" s="0" t="s">
+        <v>4046</v>
+      </c>
+      <c r="K682" s="0" t="s">
+        <v>3958</v>
+      </c>
+    </row>
+    <row r="683" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A683" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B683" s="0" t="s">
+        <v>4047</v>
+      </c>
+      <c r="C683" s="0" t="s">
+        <v>4048</v>
+      </c>
+      <c r="D683" s="0" t="s">
+        <v>4049</v>
+      </c>
+      <c r="E683" s="0" t="s">
+        <v>4050</v>
+      </c>
+      <c r="F683" s="0" t="s">
+        <v>4051</v>
+      </c>
+      <c r="G683" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I683" s="0" t="s">
+        <v>4052</v>
+      </c>
+      <c r="J683" s="0" t="s">
+        <v>4053</v>
+      </c>
+      <c r="K683" s="0" t="s">
+        <v>3949</v>
+      </c>
+    </row>
+    <row r="684" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A684" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B684" s="0" t="s">
+        <v>4054</v>
+      </c>
+      <c r="C684" s="0" t="s">
+        <v>4054</v>
+      </c>
+      <c r="D684" s="0" t="s">
+        <v>4055</v>
+      </c>
+      <c r="E684" s="0" t="s">
+        <v>4056</v>
+      </c>
+      <c r="F684" s="0" t="s">
+        <v>4057</v>
+      </c>
+      <c r="G684" s="0" t="s">
+        <v>4058</v>
+      </c>
+      <c r="I684" s="0" t="s">
+        <v>4059</v>
+      </c>
+      <c r="J684" s="0" t="s">
+        <v>4060</v>
+      </c>
+      <c r="K684" s="0" t="s">
+        <v>4013</v>
+      </c>
+    </row>
+    <row r="685" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A685" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B685" s="0" t="s">
+        <v>4061</v>
+      </c>
+      <c r="C685" s="0" t="s">
+        <v>4061</v>
+      </c>
+      <c r="D685" s="0" t="s">
+        <v>4062</v>
+      </c>
+      <c r="E685" s="0" t="s">
+        <v>4063</v>
+      </c>
+      <c r="F685" s="0" t="s">
+        <v>4064</v>
+      </c>
+      <c r="G685" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I685" s="0" t="s">
+        <v>4065</v>
+      </c>
+      <c r="J685" s="0" t="s">
+        <v>4066</v>
+      </c>
+      <c r="K685" s="0" t="s">
+        <v>3958</v>
+      </c>
+    </row>
+    <row r="686" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A686" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B686" s="0" t="s">
+        <v>4067</v>
+      </c>
+      <c r="C686" s="0" t="s">
+        <v>4068</v>
+      </c>
+      <c r="D686" s="0" t="s">
+        <v>4069</v>
+      </c>
+      <c r="E686" s="0" t="s">
+        <v>4070</v>
+      </c>
+      <c r="F686" s="0" t="s">
+        <v>4071</v>
+      </c>
+      <c r="G686" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I686" s="0" t="s">
+        <v>4072</v>
+      </c>
+      <c r="J686" s="0" t="s">
+        <v>4073</v>
+      </c>
+      <c r="K686" s="0" t="s">
+        <v>3992</v>
+      </c>
+    </row>
+    <row r="687" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A687" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B687" s="0" t="s">
+        <v>4074</v>
+      </c>
+      <c r="C687" s="0" t="s">
+        <v>4074</v>
+      </c>
+      <c r="D687" s="0" t="s">
+        <v>4075</v>
+      </c>
+      <c r="E687" s="0" t="s">
+        <v>4076</v>
+      </c>
+      <c r="F687" s="0" t="s">
+        <v>4077</v>
+      </c>
+      <c r="G687" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I687" s="0" t="s">
+        <v>4078</v>
+      </c>
+      <c r="J687" s="0" t="s">
+        <v>4079</v>
+      </c>
+      <c r="K687" s="0" t="s">
+        <v>3992</v>
+      </c>
+    </row>
+    <row r="688" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A688" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B688" s="0" t="s">
+        <v>4080</v>
+      </c>
+      <c r="C688" s="0" t="s">
+        <v>4080</v>
+      </c>
+      <c r="D688" s="0" t="s">
+        <v>4081</v>
+      </c>
+      <c r="E688" s="0" t="s">
+        <v>4082</v>
+      </c>
+      <c r="F688" s="0" t="s">
+        <v>4083</v>
+      </c>
+      <c r="G688" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="I688" s="0" t="s">
+        <v>4084</v>
+      </c>
+      <c r="J688" s="0" t="s">
+        <v>4085</v>
+      </c>
+      <c r="K688" s="0" t="s">
+        <v>3653</v>
+      </c>
+    </row>
+    <row r="689" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A689" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B689" s="0" t="s">
+        <v>4086</v>
+      </c>
+      <c r="C689" s="0" t="s">
+        <v>4086</v>
+      </c>
+      <c r="D689" s="0" t="s">
+        <v>4087</v>
+      </c>
+      <c r="E689" s="0" t="s">
+        <v>4088</v>
+      </c>
+      <c r="F689" s="0" t="s">
+        <v>4089</v>
+      </c>
+      <c r="G689" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I689" s="0" t="s">
+        <v>4090</v>
+      </c>
+      <c r="J689" s="0" t="s">
+        <v>4091</v>
+      </c>
+      <c r="K689" s="0" t="s">
+        <v>3949</v>
+      </c>
+    </row>
+    <row r="690" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A690" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B690" s="0" t="s">
+        <v>4092</v>
+      </c>
+      <c r="C690" s="0" t="s">
+        <v>4093</v>
+      </c>
+      <c r="D690" s="0" t="s">
+        <v>4094</v>
+      </c>
+      <c r="E690" s="0" t="s">
+        <v>4095</v>
+      </c>
+      <c r="F690" s="0" t="s">
+        <v>4096</v>
+      </c>
+      <c r="G690" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I690" s="0" t="s">
+        <v>4097</v>
+      </c>
+      <c r="J690" s="0" t="s">
+        <v>4098</v>
+      </c>
+      <c r="K690" s="0" t="s">
+        <v>3489</v>
+      </c>
+    </row>
+    <row r="691" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A691" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B691" s="0" t="s">
+        <v>4099</v>
+      </c>
+      <c r="C691" s="0" t="s">
+        <v>4099</v>
+      </c>
+      <c r="D691" s="0" t="s">
+        <v>4100</v>
+      </c>
+      <c r="E691" s="0" t="s">
+        <v>4101</v>
+      </c>
+      <c r="F691" s="0" t="s">
+        <v>4102</v>
+      </c>
+      <c r="G691" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I691" s="0" t="s">
+        <v>4103</v>
+      </c>
+      <c r="J691" s="0" t="s">
+        <v>4104</v>
+      </c>
+      <c r="K691" s="0" t="s">
+        <v>4013</v>
+      </c>
+    </row>
+    <row r="692" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A692" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B692" s="0" t="s">
+        <v>4105</v>
+      </c>
+      <c r="C692" s="0" t="s">
+        <v>4105</v>
+      </c>
+      <c r="D692" s="0" t="s">
+        <v>4106</v>
+      </c>
+      <c r="E692" s="0" t="s">
+        <v>4107</v>
+      </c>
+      <c r="F692" s="0" t="s">
+        <v>4108</v>
+      </c>
+      <c r="G692" s="0" t="s">
+        <v>4058</v>
+      </c>
+      <c r="I692" s="0" t="s">
+        <v>4109</v>
+      </c>
+      <c r="J692" s="0" t="s">
+        <v>4110</v>
+      </c>
+      <c r="K692" s="0" t="s">
+        <v>3653</v>
+      </c>
+    </row>
+    <row r="693" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A693" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B693" s="0" t="s">
+        <v>4111</v>
+      </c>
+      <c r="C693" s="0" t="s">
+        <v>4112</v>
+      </c>
+      <c r="D693" s="0" t="s">
+        <v>4113</v>
+      </c>
+      <c r="E693" s="0" t="s">
+        <v>4114</v>
+      </c>
+      <c r="F693" s="0" t="s">
+        <v>4115</v>
+      </c>
+      <c r="G693" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I693" s="0" t="s">
+        <v>4116</v>
+      </c>
+      <c r="J693" s="0" t="s">
+        <v>4117</v>
+      </c>
+      <c r="K693" s="0" t="s">
+        <v>3489</v>
+      </c>
+    </row>
+    <row r="694" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A694" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B694" s="0" t="s">
+        <v>4118</v>
+      </c>
+      <c r="C694" s="0" t="s">
+        <v>4118</v>
+      </c>
+      <c r="D694" s="0" t="s">
+        <v>4119</v>
+      </c>
+      <c r="E694" s="0" t="s">
+        <v>4120</v>
+      </c>
+      <c r="F694" s="0" t="s">
+        <v>4121</v>
+      </c>
+      <c r="G694" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I694" s="0" t="s">
+        <v>4122</v>
+      </c>
+      <c r="J694" s="0" t="s">
+        <v>4123</v>
+      </c>
+      <c r="K694" s="0" t="s">
+        <v>3489</v>
+      </c>
+    </row>
+    <row r="695" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A695" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B695" s="0" t="s">
+        <v>4124</v>
+      </c>
+      <c r="C695" s="0" t="s">
+        <v>4125</v>
+      </c>
+      <c r="D695" s="0" t="s">
+        <v>4126</v>
+      </c>
+      <c r="E695" s="0" t="s">
+        <v>4127</v>
+      </c>
+      <c r="F695" s="0" t="s">
+        <v>4128</v>
+      </c>
+      <c r="G695" s="0" t="s">
+        <v>418</v>
+      </c>
+      <c r="I695" s="0" t="s">
+        <v>4129</v>
+      </c>
+      <c r="J695" s="0" t="s">
+        <v>4130</v>
+      </c>
+      <c r="K695" s="0" t="s">
+        <v>3992</v>
+      </c>
+    </row>
+    <row r="696" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A696" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B696" s="0" t="s">
+        <v>4131</v>
+      </c>
+      <c r="C696" s="0" t="s">
+        <v>4132</v>
+      </c>
+      <c r="D696" s="0" t="s">
+        <v>4133</v>
+      </c>
+      <c r="E696" s="0" t="s">
+        <v>4134</v>
+      </c>
+      <c r="F696" s="0" t="s">
+        <v>4135</v>
+      </c>
+      <c r="G696" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I696" s="0" t="s">
+        <v>3956</v>
+      </c>
+      <c r="J696" s="0" t="s">
+        <v>3957</v>
+      </c>
+      <c r="K696" s="0" t="s">
+        <v>3958</v>
+      </c>
+    </row>
+    <row r="697" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A697" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B697" s="0" t="s">
+        <v>4136</v>
+      </c>
+      <c r="C697" s="0" t="s">
+        <v>4137</v>
+      </c>
+      <c r="D697" s="0" t="s">
+        <v>4138</v>
+      </c>
+      <c r="E697" s="0" t="s">
+        <v>4139</v>
+      </c>
+      <c r="F697" s="0" t="s">
+        <v>4140</v>
+      </c>
+      <c r="G697" s="0" t="s">
+        <v>4141</v>
+      </c>
+      <c r="I697" s="0" t="s">
+        <v>4142</v>
+      </c>
+      <c r="J697" s="0" t="s">
+        <v>4143</v>
+      </c>
+      <c r="K697" s="0" t="s">
+        <v>3949</v>
+      </c>
+    </row>
+    <row r="698" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A698" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B698" s="0" t="s">
+        <v>4144</v>
+      </c>
+      <c r="C698" s="0" t="s">
+        <v>4144</v>
+      </c>
+      <c r="D698" s="0" t="s">
+        <v>4145</v>
+      </c>
+      <c r="E698" s="0" t="s">
+        <v>4146</v>
+      </c>
+      <c r="F698" s="0" t="s">
+        <v>4147</v>
+      </c>
+      <c r="G698" s="0" t="s">
+        <v>4148</v>
+      </c>
+      <c r="I698" s="0" t="s">
+        <v>4149</v>
+      </c>
+      <c r="J698" s="0" t="s">
+        <v>4150</v>
+      </c>
+      <c r="K698" s="0" t="s">
+        <v>3653</v>
+      </c>
+    </row>
+    <row r="699" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A699" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B699" s="0" t="s">
+        <v>4151</v>
+      </c>
+      <c r="C699" s="0" t="s">
+        <v>4152</v>
+      </c>
+      <c r="D699" s="0" t="s">
+        <v>4153</v>
+      </c>
+      <c r="E699" s="0" t="s">
+        <v>4154</v>
+      </c>
+      <c r="F699" s="0" t="s">
+        <v>4155</v>
+      </c>
+      <c r="G699" s="0" t="s">
+        <v>418</v>
+      </c>
+      <c r="I699" s="0" t="s">
+        <v>4156</v>
+      </c>
+      <c r="J699" s="0" t="s">
+        <v>4157</v>
+      </c>
+      <c r="K699" s="0" t="s">
+        <v>4013</v>
+      </c>
+    </row>
+    <row r="700" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A700" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B700" s="0" t="s">
+        <v>4158</v>
+      </c>
+      <c r="C700" s="0" t="s">
+        <v>4159</v>
+      </c>
+      <c r="D700" s="0" t="s">
+        <v>4160</v>
+      </c>
+      <c r="E700" s="0" t="s">
+        <v>4161</v>
+      </c>
+      <c r="F700" s="0" t="s">
+        <v>4162</v>
+      </c>
+      <c r="G700" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="I700" s="0" t="s">
+        <v>4163</v>
+      </c>
+      <c r="J700" s="0" t="s">
+        <v>4164</v>
+      </c>
+      <c r="K700" s="0" t="s">
+        <v>3653</v>
+      </c>
+    </row>
+    <row r="701" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A701" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B701" s="0" t="s">
+        <v>4165</v>
+      </c>
+      <c r="C701" s="0" t="s">
+        <v>4166</v>
+      </c>
+      <c r="D701" s="0" t="s">
+        <v>4167</v>
+      </c>
+      <c r="E701" s="0" t="s">
+        <v>4168</v>
+      </c>
+      <c r="F701" s="0" t="s">
+        <v>4169</v>
+      </c>
+      <c r="G701" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="I701" s="0" t="s">
+        <v>4170</v>
+      </c>
+      <c r="J701" s="0" t="s">
+        <v>4171</v>
+      </c>
+      <c r="K701" s="0" t="s">
+        <v>3958</v>
+      </c>
+    </row>
+    <row r="702" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A702" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B702" s="0" t="s">
+        <v>4172</v>
+      </c>
+      <c r="C702" s="0" t="s">
+        <v>4173</v>
+      </c>
+      <c r="D702" s="0" t="s">
+        <v>4174</v>
+      </c>
+      <c r="E702" s="0" t="s">
+        <v>4175</v>
+      </c>
+      <c r="F702" s="0" t="s">
+        <v>4176</v>
+      </c>
+      <c r="G702" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I702" s="0" t="s">
+        <v>4177</v>
+      </c>
+      <c r="J702" s="0" t="s">
+        <v>4178</v>
+      </c>
+      <c r="K702" s="0" t="s">
+        <v>3489</v>
+      </c>
+    </row>
+    <row r="703" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A703" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B703" s="0" t="s">
+        <v>4179</v>
+      </c>
+      <c r="C703" s="0" t="s">
+        <v>4180</v>
+      </c>
+      <c r="D703" s="0" t="s">
+        <v>4181</v>
+      </c>
+      <c r="E703" s="0" t="s">
+        <v>4182</v>
+      </c>
+      <c r="F703" s="0" t="s">
+        <v>4183</v>
+      </c>
+      <c r="G703" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I703" s="0" t="s">
+        <v>4184</v>
+      </c>
+      <c r="J703" s="0" t="s">
+        <v>4185</v>
+      </c>
+      <c r="K703" s="0" t="s">
+        <v>3992</v>
+      </c>
+    </row>
+    <row r="704" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A704" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B704" s="0" t="s">
+        <v>4186</v>
+      </c>
+      <c r="C704" s="0" t="s">
+        <v>4187</v>
+      </c>
+      <c r="D704" s="0" t="s">
+        <v>4188</v>
+      </c>
+      <c r="E704" s="0" t="s">
+        <v>4187</v>
+      </c>
+      <c r="F704" s="0" t="s">
+        <v>4189</v>
+      </c>
+      <c r="G704" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I704" s="0" t="s">
+        <v>3956</v>
+      </c>
+      <c r="J704" s="0" t="s">
+        <v>3957</v>
+      </c>
+      <c r="K704" s="0" t="s">
+        <v>3958</v>
+      </c>
+    </row>
+    <row r="705" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A705" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B705" s="0" t="s">
+        <v>4190</v>
+      </c>
+      <c r="C705" s="0" t="s">
+        <v>4191</v>
+      </c>
+      <c r="D705" s="0" t="s">
+        <v>4192</v>
+      </c>
+      <c r="E705" s="0" t="s">
+        <v>4193</v>
+      </c>
+      <c r="F705" s="0" t="s">
+        <v>4194</v>
+      </c>
+      <c r="G705" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I705" s="0" t="s">
+        <v>3977</v>
+      </c>
+      <c r="J705" s="0" t="s">
+        <v>3978</v>
+      </c>
+      <c r="K705" s="0" t="s">
+        <v>3958</v>
+      </c>
+    </row>
+    <row r="706" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A706" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B706" s="0" t="s">
+        <v>4195</v>
+      </c>
+      <c r="C706" s="0" t="s">
+        <v>4195</v>
+      </c>
+      <c r="D706" s="0" t="s">
+        <v>4196</v>
+      </c>
+      <c r="E706" s="0" t="s">
+        <v>4197</v>
+      </c>
+      <c r="F706" s="0" t="s">
+        <v>4198</v>
+      </c>
+      <c r="G706" s="0" t="s">
+        <v>4199</v>
+      </c>
+      <c r="I706" s="0" t="s">
+        <v>4200</v>
+      </c>
+      <c r="J706" s="0" t="s">
+        <v>4201</v>
+      </c>
+      <c r="K706" s="0" t="s">
+        <v>3992</v>
+      </c>
+    </row>
+    <row r="707" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A707" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B707" s="0" t="s">
+        <v>4202</v>
+      </c>
+      <c r="C707" s="0" t="s">
+        <v>4202</v>
+      </c>
+      <c r="D707" s="0" t="s">
+        <v>4203</v>
+      </c>
+      <c r="E707" s="0" t="s">
+        <v>4204</v>
+      </c>
+      <c r="F707" s="0" t="s">
+        <v>4205</v>
+      </c>
+      <c r="G707" s="0" t="s">
+        <v>4206</v>
+      </c>
+      <c r="I707" s="0" t="s">
+        <v>4207</v>
+      </c>
+      <c r="J707" s="0" t="s">
+        <v>4208</v>
+      </c>
+      <c r="K707" s="0" t="s">
+        <v>3949</v>
+      </c>
+    </row>
+    <row r="708" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A708" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B708" s="0" t="s">
+        <v>4209</v>
+      </c>
+      <c r="C708" s="0" t="s">
+        <v>4210</v>
+      </c>
+      <c r="D708" s="0" t="s">
+        <v>4211</v>
+      </c>
+      <c r="E708" s="0" t="s">
+        <v>4212</v>
+      </c>
+      <c r="F708" s="0" t="s">
+        <v>4213</v>
+      </c>
+      <c r="G708" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I708" s="0" t="s">
+        <v>4065</v>
+      </c>
+      <c r="J708" s="0" t="s">
+        <v>4066</v>
+      </c>
+      <c r="K708" s="0" t="s">
+        <v>3958</v>
+      </c>
+    </row>
+    <row r="709" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A709" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B709" s="0" t="s">
+        <v>4214</v>
+      </c>
+      <c r="C709" s="0" t="s">
+        <v>4215</v>
+      </c>
+      <c r="D709" s="0" t="s">
+        <v>4216</v>
+      </c>
+      <c r="E709" s="0" t="s">
+        <v>4217</v>
+      </c>
+      <c r="F709" s="0" t="s">
+        <v>4218</v>
+      </c>
+      <c r="G709" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I709" s="0" t="s">
+        <v>3956</v>
+      </c>
+      <c r="J709" s="0" t="s">
+        <v>3957</v>
+      </c>
+      <c r="K709" s="0" t="s">
+        <v>3958</v>
+      </c>
+    </row>
+    <row r="710" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A710" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B710" s="0" t="s">
+        <v>4219</v>
+      </c>
+      <c r="C710" s="0" t="s">
+        <v>4219</v>
+      </c>
+      <c r="D710" s="0" t="s">
+        <v>4220</v>
+      </c>
+      <c r="E710" s="0" t="s">
+        <v>4221</v>
+      </c>
+      <c r="F710" s="0" t="s">
+        <v>4222</v>
+      </c>
+      <c r="G710" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I710" s="0" t="s">
+        <v>4223</v>
+      </c>
+      <c r="J710" s="0" t="s">
+        <v>4224</v>
+      </c>
+      <c r="K710" s="0" t="s">
+        <v>3949</v>
+      </c>
+    </row>
+    <row r="711" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A711" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B711" s="0" t="s">
+        <v>4225</v>
+      </c>
+      <c r="C711" s="0" t="s">
+        <v>4225</v>
+      </c>
+      <c r="D711" s="0" t="s">
+        <v>4226</v>
+      </c>
+      <c r="E711" s="0" t="s">
+        <v>4227</v>
+      </c>
+      <c r="F711" s="0" t="s">
+        <v>4228</v>
+      </c>
+      <c r="G711" s="0" t="s">
+        <v>4229</v>
+      </c>
+      <c r="I711" s="0" t="s">
+        <v>4200</v>
+      </c>
+      <c r="J711" s="0" t="s">
+        <v>4201</v>
+      </c>
+      <c r="K711" s="0" t="s">
+        <v>3992</v>
+      </c>
+    </row>
+    <row r="712" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A712" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B712" s="0" t="s">
+        <v>4230</v>
+      </c>
+      <c r="C712" s="0" t="s">
+        <v>4231</v>
+      </c>
+      <c r="D712" s="0" t="s">
+        <v>4232</v>
+      </c>
+      <c r="E712" s="0" t="s">
+        <v>4233</v>
+      </c>
+      <c r="F712" s="0" t="s">
+        <v>4234</v>
+      </c>
+      <c r="G712" s="0" t="s">
+        <v>418</v>
+      </c>
+      <c r="I712" s="0" t="s">
+        <v>4235</v>
+      </c>
+      <c r="J712" s="0" t="s">
+        <v>4236</v>
+      </c>
+      <c r="K712" s="0" t="s">
+        <v>3958</v>
+      </c>
+    </row>
+    <row r="713" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A713" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B713" s="0" t="s">
+        <v>4237</v>
+      </c>
+      <c r="C713" s="0" t="s">
+        <v>4238</v>
+      </c>
+      <c r="D713" s="0" t="s">
+        <v>4239</v>
+      </c>
+      <c r="E713" s="0" t="s">
+        <v>4240</v>
+      </c>
+      <c r="F713" s="0" t="s">
+        <v>4241</v>
+      </c>
+      <c r="G713" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I713" s="0" t="s">
+        <v>4184</v>
+      </c>
+      <c r="J713" s="0" t="s">
+        <v>4185</v>
+      </c>
+      <c r="K713" s="0" t="s">
+        <v>3992</v>
+      </c>
+    </row>
+    <row r="714" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A714" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B714" s="0" t="s">
+        <v>4242</v>
+      </c>
+      <c r="C714" s="0" t="s">
+        <v>4243</v>
+      </c>
+      <c r="D714" s="0" t="s">
+        <v>4244</v>
+      </c>
+      <c r="E714" s="0" t="s">
+        <v>4245</v>
+      </c>
+      <c r="F714" s="0" t="s">
+        <v>4246</v>
+      </c>
+      <c r="G714" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I714" s="0" t="s">
+        <v>4247</v>
+      </c>
+      <c r="J714" s="0" t="s">
+        <v>4248</v>
+      </c>
+      <c r="K714" s="0" t="s">
+        <v>3992</v>
+      </c>
+    </row>
+    <row r="715" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A715" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B715" s="0" t="s">
+        <v>4249</v>
+      </c>
+      <c r="C715" s="0" t="s">
+        <v>4249</v>
+      </c>
+      <c r="D715" s="0" t="s">
+        <v>4250</v>
+      </c>
+      <c r="E715" s="0" t="s">
+        <v>4251</v>
+      </c>
+      <c r="F715" s="0" t="s">
+        <v>4252</v>
+      </c>
+      <c r="G715" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I715" s="0" t="s">
+        <v>4200</v>
+      </c>
+      <c r="J715" s="0" t="s">
+        <v>4201</v>
+      </c>
+      <c r="K715" s="0" t="s">
+        <v>3992</v>
+      </c>
+    </row>
+    <row r="716" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A716" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B716" s="0" t="s">
+        <v>4253</v>
+      </c>
+      <c r="C716" s="0" t="s">
+        <v>4254</v>
+      </c>
+      <c r="D716" s="0" t="s">
+        <v>4255</v>
+      </c>
+      <c r="E716" s="0" t="s">
+        <v>4256</v>
+      </c>
+      <c r="F716" s="0" t="s">
+        <v>4257</v>
+      </c>
+      <c r="G716" s="0" t="s">
+        <v>4258</v>
+      </c>
+      <c r="H716" s="0" t="s">
+        <v>764</v>
+      </c>
+      <c r="I716" s="0" t="s">
+        <v>4259</v>
+      </c>
+      <c r="J716" s="0" t="s">
+        <v>4260</v>
+      </c>
+      <c r="K716" s="0" t="s">
+        <v>3992</v>
+      </c>
+    </row>
+    <row r="717" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A717" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B717" s="0" t="s">
+        <v>4261</v>
+      </c>
+      <c r="C717" s="0" t="s">
+        <v>4261</v>
+      </c>
+      <c r="D717" s="0" t="s">
+        <v>4262</v>
+      </c>
+      <c r="E717" s="0" t="s">
+        <v>4263</v>
+      </c>
+      <c r="F717" s="0" t="s">
+        <v>4264</v>
+      </c>
+      <c r="G717" s="0" t="s">
+        <v>4265</v>
+      </c>
+      <c r="H717" s="0" t="s">
+        <v>3936</v>
+      </c>
+      <c r="I717" s="0" t="s">
+        <v>4266</v>
+      </c>
+      <c r="J717" s="0" t="s">
+        <v>4267</v>
+      </c>
+      <c r="K717" s="0" t="s">
+        <v>3949</v>
+      </c>
+    </row>
+    <row r="718" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A718" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B718" s="0" t="s">
+        <v>4268</v>
+      </c>
+      <c r="C718" s="0" t="s">
+        <v>4268</v>
+      </c>
+      <c r="D718" s="0" t="s">
+        <v>4269</v>
+      </c>
+      <c r="E718" s="0" t="s">
+        <v>4256</v>
+      </c>
+      <c r="F718" s="0" t="s">
+        <v>4257</v>
+      </c>
+      <c r="G718" s="0" t="s">
+        <v>4258</v>
+      </c>
+      <c r="H718" s="0" t="s">
+        <v>1296</v>
+      </c>
+      <c r="I718" s="0" t="s">
+        <v>4259</v>
+      </c>
+      <c r="J718" s="0" t="s">
+        <v>4260</v>
+      </c>
+      <c r="K718" s="0" t="s">
+        <v>3992</v>
+      </c>
+    </row>
+    <row r="719" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A719" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B719" s="0" t="s">
+        <v>4270</v>
+      </c>
+      <c r="C719" s="0" t="s">
+        <v>4271</v>
+      </c>
+      <c r="D719" s="0" t="s">
+        <v>4272</v>
+      </c>
+      <c r="E719" s="0" t="s">
+        <v>4273</v>
+      </c>
+      <c r="F719" s="0" t="s">
+        <v>4274</v>
+      </c>
+      <c r="G719" s="0" t="s">
+        <v>4275</v>
+      </c>
+      <c r="H719" s="0" t="s">
+        <v>911</v>
+      </c>
+      <c r="I719" s="0" t="s">
+        <v>4276</v>
+      </c>
+      <c r="J719" s="0" t="s">
+        <v>4277</v>
+      </c>
+      <c r="K719" s="0" t="s">
+        <v>4013</v>
+      </c>
+    </row>
+    <row r="720" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A720" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B720" s="0" t="s">
+        <v>4278</v>
+      </c>
+      <c r="C720" s="0" t="s">
+        <v>4279</v>
+      </c>
+      <c r="D720" s="0" t="s">
+        <v>4280</v>
+      </c>
+      <c r="E720" s="0" t="s">
+        <v>4281</v>
+      </c>
+      <c r="F720" s="0" t="s">
+        <v>4282</v>
+      </c>
+      <c r="G720" s="0" t="s">
+        <v>4283</v>
+      </c>
+      <c r="H720" s="0" t="s">
+        <v>609</v>
+      </c>
+      <c r="I720" s="0" t="s">
+        <v>3984</v>
+      </c>
+      <c r="J720" s="0" t="s">
+        <v>3985</v>
+      </c>
+      <c r="K720" s="0" t="s">
+        <v>3489</v>
+      </c>
+    </row>
+    <row r="721" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A721" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B721" s="0" t="s">
+        <v>4284</v>
+      </c>
+      <c r="C721" s="0" t="s">
+        <v>3077</v>
+      </c>
+      <c r="D721" s="0" t="s">
+        <v>3078</v>
+      </c>
+      <c r="E721" s="0" t="s">
+        <v>3079</v>
+      </c>
+      <c r="F721" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="G721" s="0" t="s">
+        <v>4285</v>
+      </c>
+      <c r="H721" s="0" t="s">
+        <v>1296</v>
+      </c>
+      <c r="I721" s="0" t="s">
+        <v>4286</v>
+      </c>
+      <c r="J721" s="0" t="s">
+        <v>4287</v>
+      </c>
+      <c r="K721" s="0" t="s">
+        <v>4013</v>
+      </c>
+    </row>
+    <row r="722" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A722" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B722" s="0" t="s">
+        <v>4288</v>
+      </c>
+      <c r="C722" s="0" t="s">
+        <v>4288</v>
+      </c>
+      <c r="D722" s="0" t="s">
+        <v>4289</v>
+      </c>
+      <c r="E722" s="0" t="s">
+        <v>4290</v>
+      </c>
+      <c r="F722" s="0" t="s">
+        <v>4291</v>
+      </c>
+      <c r="G722" s="0" t="s">
+        <v>4292</v>
+      </c>
+      <c r="H722" s="0" t="s">
+        <v>4293</v>
+      </c>
+      <c r="I722" s="0" t="s">
+        <v>4294</v>
+      </c>
+      <c r="J722" s="0" t="s">
+        <v>4295</v>
+      </c>
+      <c r="K722" s="0" t="s">
+        <v>3958</v>
+      </c>
+    </row>
+    <row r="723" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A723" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B723" s="0" t="s">
+        <v>4296</v>
+      </c>
+      <c r="C723" s="0" t="s">
+        <v>4296</v>
+      </c>
+      <c r="D723" s="0" t="s">
+        <v>4297</v>
+      </c>
+      <c r="E723" s="0" t="s">
+        <v>4298</v>
+      </c>
+      <c r="F723" s="0" t="s">
+        <v>4299</v>
+      </c>
+      <c r="G723" s="0" t="s">
+        <v>4265</v>
+      </c>
+      <c r="H723" s="0" t="s">
+        <v>4300</v>
+      </c>
+      <c r="I723" s="0" t="s">
+        <v>4301</v>
+      </c>
+      <c r="J723" s="0" t="s">
+        <v>4302</v>
+      </c>
+      <c r="K723" s="0" t="s">
+        <v>4013</v>
+      </c>
+    </row>
+    <row r="724" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A724" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B724" s="0" t="s">
+        <v>4303</v>
+      </c>
+      <c r="C724" s="0" t="s">
+        <v>4304</v>
+      </c>
+      <c r="D724" s="0" t="s">
+        <v>4305</v>
+      </c>
+      <c r="E724" s="0" t="s">
+        <v>4306</v>
+      </c>
+      <c r="F724" s="0" t="s">
+        <v>4307</v>
+      </c>
+      <c r="G724" s="0" t="s">
+        <v>4258</v>
+      </c>
+      <c r="H724" s="0" t="s">
+        <v>764</v>
+      </c>
+      <c r="I724" s="0" t="s">
+        <v>4308</v>
+      </c>
+      <c r="J724" s="0" t="s">
+        <v>4309</v>
+      </c>
+      <c r="K724" s="0" t="s">
+        <v>3958</v>
+      </c>
+    </row>
+    <row r="725" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A725" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B725" s="0" t="s">
+        <v>4310</v>
+      </c>
+      <c r="C725" s="0" t="s">
+        <v>4311</v>
+      </c>
+      <c r="D725" s="0" t="s">
+        <v>4312</v>
+      </c>
+      <c r="E725" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="F725" s="0" t="s">
+        <v>3152</v>
+      </c>
+      <c r="G725" s="0" t="s">
+        <v>4258</v>
+      </c>
+      <c r="H725" s="0" t="s">
+        <v>764</v>
+      </c>
+      <c r="I725" s="0" t="s">
+        <v>4313</v>
+      </c>
+      <c r="J725" s="0" t="s">
+        <v>4314</v>
+      </c>
+      <c r="K725" s="0" t="s">
+        <v>3949</v>
+      </c>
+    </row>
+    <row r="726" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A726" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B726" s="0" t="s">
+        <v>4315</v>
+      </c>
+      <c r="C726" s="0" t="s">
+        <v>3192</v>
+      </c>
+      <c r="D726" s="0" t="s">
+        <v>3193</v>
+      </c>
+      <c r="E726" s="0" t="s">
+        <v>3194</v>
+      </c>
+      <c r="F726" s="0" t="s">
+        <v>3195</v>
+      </c>
+      <c r="G726" s="0" t="s">
+        <v>4316</v>
+      </c>
+      <c r="H726" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="I726" s="0" t="s">
+        <v>4317</v>
+      </c>
+      <c r="J726" s="0" t="s">
+        <v>4318</v>
+      </c>
+      <c r="K726" s="0" t="s">
+        <v>3992</v>
+      </c>
+    </row>
+    <row r="727" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A727" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B727" s="0" t="s">
+        <v>4319</v>
+      </c>
+      <c r="C727" s="0" t="s">
+        <v>4320</v>
+      </c>
+      <c r="D727" s="0" t="s">
+        <v>4321</v>
+      </c>
+      <c r="E727" s="0" t="s">
+        <v>4322</v>
+      </c>
+      <c r="F727" s="0" t="s">
+        <v>4323</v>
+      </c>
+      <c r="G727" s="0" t="s">
+        <v>4285</v>
+      </c>
+      <c r="H727" s="0" t="s">
+        <v>2151</v>
+      </c>
+      <c r="I727" s="0" t="s">
+        <v>3984</v>
+      </c>
+      <c r="J727" s="0" t="s">
+        <v>3985</v>
+      </c>
+      <c r="K727" s="0" t="s">
+        <v>3489</v>
+      </c>
+    </row>
+    <row r="728" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A728" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B728" s="0" t="s">
+        <v>1526</v>
+      </c>
+      <c r="C728" s="0" t="s">
+        <v>1527</v>
+      </c>
+      <c r="D728" s="0" t="s">
+        <v>1528</v>
+      </c>
+      <c r="E728" s="0" t="s">
+        <v>1529</v>
+      </c>
+      <c r="F728" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="G728" s="0" t="s">
+        <v>4316</v>
+      </c>
+      <c r="H728" s="0" t="s">
+        <v>1530</v>
+      </c>
+      <c r="I728" s="0" t="s">
+        <v>4324</v>
+      </c>
+      <c r="J728" s="0" t="s">
+        <v>4325</v>
+      </c>
+      <c r="K728" s="0" t="s">
+        <v>3949</v>
+      </c>
+    </row>
+    <row r="729" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A729" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B729" s="0" t="s">
+        <v>4326</v>
+      </c>
+      <c r="C729" s="0" t="s">
+        <v>4327</v>
+      </c>
+      <c r="D729" s="0" t="s">
+        <v>4328</v>
+      </c>
+      <c r="E729" s="1" t="s">
+        <v>4329</v>
+      </c>
+      <c r="F729" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="G729" s="0" t="s">
+        <v>4316</v>
+      </c>
+      <c r="H729" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="I729" s="0" t="s">
+        <v>4330</v>
+      </c>
+      <c r="J729" s="0" t="s">
+        <v>4331</v>
+      </c>
+      <c r="K729" s="0" t="s">
+        <v>3489</v>
+      </c>
+      <c r="L729" s="0" t="s">
+        <v>4332</v>
+      </c>
+    </row>
+    <row r="730" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A730" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B730" s="0" t="s">
+        <v>4333</v>
+      </c>
+      <c r="C730" s="0" t="s">
+        <v>4334</v>
+      </c>
+      <c r="D730" s="0" t="s">
+        <v>4335</v>
+      </c>
+      <c r="E730" s="0" t="s">
+        <v>4336</v>
+      </c>
+      <c r="F730" s="0" t="s">
+        <v>2076</v>
+      </c>
+      <c r="G730" s="0" t="s">
+        <v>4285</v>
+      </c>
+      <c r="H730" s="0" t="s">
+        <v>803</v>
+      </c>
+      <c r="I730" s="0" t="s">
+        <v>4103</v>
+      </c>
+      <c r="J730" s="0" t="s">
+        <v>4104</v>
+      </c>
+      <c r="K730" s="0" t="s">
+        <v>4013</v>
+      </c>
+    </row>
+    <row r="731" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A731" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B731" s="0" t="s">
+        <v>4337</v>
+      </c>
+      <c r="C731" s="0" t="s">
+        <v>4338</v>
+      </c>
+      <c r="D731" s="0" t="s">
+        <v>4339</v>
+      </c>
+      <c r="E731" s="0" t="s">
+        <v>4340</v>
+      </c>
+      <c r="F731" s="0" t="s">
+        <v>4341</v>
+      </c>
+      <c r="G731" s="0" t="s">
+        <v>4342</v>
+      </c>
+      <c r="H731" s="0" t="s">
+        <v>2214</v>
+      </c>
+      <c r="I731" s="0" t="s">
+        <v>4343</v>
+      </c>
+      <c r="J731" s="0" t="s">
+        <v>4344</v>
+      </c>
+      <c r="K731" s="0" t="s">
+        <v>4013</v>
+      </c>
+    </row>
+    <row r="732" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A732" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B732" s="0" t="s">
+        <v>4345</v>
+      </c>
+      <c r="C732" s="0" t="s">
+        <v>4346</v>
+      </c>
+      <c r="D732" s="0" t="s">
+        <v>4347</v>
+      </c>
+      <c r="E732" s="0" t="s">
+        <v>4348</v>
+      </c>
+      <c r="F732" s="0" t="s">
+        <v>4349</v>
+      </c>
+      <c r="G732" s="0" t="s">
+        <v>4258</v>
+      </c>
+      <c r="H732" s="0" t="s">
+        <v>4350</v>
+      </c>
+      <c r="I732" s="0" t="s">
+        <v>4059</v>
+      </c>
+      <c r="J732" s="0" t="s">
+        <v>4060</v>
+      </c>
+      <c r="K732" s="0" t="s">
+        <v>4013</v>
+      </c>
+    </row>
+    <row r="733" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A733" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B733" s="0" t="s">
+        <v>4351</v>
+      </c>
+      <c r="C733" s="0" t="s">
+        <v>4352</v>
+      </c>
+      <c r="D733" s="0" t="s">
+        <v>4353</v>
+      </c>
+      <c r="E733" s="0" t="s">
+        <v>4354</v>
+      </c>
+      <c r="F733" s="0" t="s">
+        <v>4355</v>
+      </c>
+      <c r="G733" s="0" t="s">
+        <v>4285</v>
+      </c>
+      <c r="H733" s="0" t="s">
+        <v>4356</v>
+      </c>
+      <c r="I733" s="0" t="s">
+        <v>4357</v>
+      </c>
+      <c r="J733" s="0" t="s">
+        <v>4358</v>
+      </c>
+      <c r="K733" s="0" t="s">
+        <v>3489</v>
+      </c>
+    </row>
+    <row r="734" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A734" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B734" s="0" t="s">
+        <v>4359</v>
+      </c>
+      <c r="C734" s="0" t="s">
+        <v>4360</v>
+      </c>
+      <c r="D734" s="0" t="s">
+        <v>4361</v>
+      </c>
+      <c r="E734" s="0" t="s">
+        <v>2757</v>
+      </c>
+      <c r="F734" s="0" t="s">
+        <v>2758</v>
+      </c>
+      <c r="G734" s="0" t="s">
+        <v>4316</v>
+      </c>
+      <c r="H734" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="I734" s="0" t="s">
+        <v>4362</v>
+      </c>
+      <c r="J734" s="0" t="s">
+        <v>4363</v>
+      </c>
+      <c r="K734" s="0" t="s">
+        <v>3949</v>
+      </c>
+    </row>
+    <row r="735" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A735" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B735" s="0" t="s">
+        <v>4364</v>
+      </c>
+      <c r="C735" s="0" t="s">
+        <v>4364</v>
+      </c>
+      <c r="D735" s="0" t="s">
+        <v>4365</v>
+      </c>
+      <c r="E735" s="0" t="s">
+        <v>2120</v>
+      </c>
+      <c r="F735" s="0" t="s">
+        <v>2119</v>
+      </c>
+      <c r="G735" s="0" t="s">
+        <v>4366</v>
+      </c>
+      <c r="H735" s="0" t="s">
+        <v>4367</v>
+      </c>
+      <c r="I735" s="0" t="s">
+        <v>4368</v>
+      </c>
+      <c r="J735" s="0" t="s">
+        <v>4369</v>
+      </c>
+      <c r="K735" s="0" t="s">
+        <v>3958</v>
+      </c>
+    </row>
+    <row r="736" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A736" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B736" s="0" t="s">
+        <v>4370</v>
+      </c>
+      <c r="C736" s="0" t="s">
+        <v>4371</v>
+      </c>
+      <c r="D736" s="0" t="s">
+        <v>4372</v>
+      </c>
+      <c r="E736" s="0" t="s">
+        <v>4373</v>
+      </c>
+      <c r="F736" s="0" t="s">
+        <v>4374</v>
+      </c>
+      <c r="G736" s="0" t="s">
+        <v>4258</v>
+      </c>
+      <c r="H736" s="0" t="s">
+        <v>1876</v>
+      </c>
+      <c r="I736" s="0" t="s">
+        <v>4005</v>
+      </c>
+      <c r="J736" s="0" t="s">
+        <v>4006</v>
+      </c>
+      <c r="K736" s="0" t="s">
+        <v>3949</v>
+      </c>
+    </row>
+    <row r="737" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A737" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B737" s="0" t="s">
+        <v>4375</v>
+      </c>
+      <c r="C737" s="0" t="s">
+        <v>4375</v>
+      </c>
+      <c r="D737" s="0" t="s">
+        <v>4376</v>
+      </c>
+      <c r="E737" s="0" t="s">
+        <v>4377</v>
+      </c>
+      <c r="F737" s="0" t="s">
+        <v>4378</v>
+      </c>
+      <c r="G737" s="0" t="s">
+        <v>4265</v>
+      </c>
+      <c r="H737" s="0" t="s">
+        <v>3936</v>
+      </c>
+      <c r="I737" s="0" t="s">
+        <v>4379</v>
+      </c>
+      <c r="J737" s="0" t="s">
+        <v>4380</v>
+      </c>
+      <c r="K737" s="0" t="s">
+        <v>3992</v>
+      </c>
+    </row>
+    <row r="738" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A738" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B738" s="0" t="s">
+        <v>4381</v>
+      </c>
+      <c r="C738" s="0" t="s">
+        <v>4381</v>
+      </c>
+      <c r="D738" s="0" t="s">
+        <v>4382</v>
+      </c>
+      <c r="E738" s="0" t="s">
+        <v>3322</v>
+      </c>
+      <c r="F738" s="0" t="s">
+        <v>3323</v>
+      </c>
+      <c r="G738" s="0" t="s">
+        <v>4383</v>
+      </c>
+      <c r="H738" s="0" t="s">
+        <v>1194</v>
+      </c>
+      <c r="I738" s="0" t="s">
+        <v>4384</v>
+      </c>
+      <c r="J738" s="0" t="s">
+        <v>4385</v>
+      </c>
+      <c r="K738" s="0" t="s">
+        <v>3949</v>
+      </c>
+    </row>
+    <row r="739" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A739" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B739" s="0" t="s">
+        <v>4386</v>
+      </c>
+      <c r="C739" s="0" t="s">
+        <v>4387</v>
+      </c>
+      <c r="D739" s="0" t="s">
+        <v>4388</v>
+      </c>
+      <c r="E739" s="0" t="s">
+        <v>3322</v>
+      </c>
+      <c r="F739" s="0" t="s">
+        <v>3323</v>
+      </c>
+      <c r="G739" s="0" t="s">
+        <v>4316</v>
+      </c>
+      <c r="H739" s="0" t="s">
+        <v>609</v>
+      </c>
+      <c r="I739" s="0" t="s">
+        <v>4384</v>
+      </c>
+      <c r="J739" s="0" t="s">
+        <v>4385</v>
+      </c>
+      <c r="K739" s="0" t="s">
+        <v>3949</v>
+      </c>
+    </row>
+    <row r="740" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A740" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B740" s="0" t="s">
+        <v>4389</v>
+      </c>
+      <c r="C740" s="0" t="s">
+        <v>871</v>
+      </c>
+      <c r="D740" s="0" t="s">
+        <v>872</v>
+      </c>
+      <c r="E740" s="0" t="s">
+        <v>873</v>
+      </c>
+      <c r="F740" s="0" t="s">
+        <v>874</v>
+      </c>
+      <c r="G740" s="0" t="s">
+        <v>4316</v>
+      </c>
+      <c r="H740" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="I740" s="0" t="s">
+        <v>4390</v>
+      </c>
+      <c r="J740" s="0" t="s">
+        <v>4391</v>
+      </c>
+      <c r="K740" s="0" t="s">
+        <v>3949</v>
+      </c>
+    </row>
+    <row r="741" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A741" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B741" s="0" t="s">
+        <v>4392</v>
+      </c>
+      <c r="C741" s="0" t="s">
+        <v>4393</v>
+      </c>
+      <c r="D741" s="0" t="s">
+        <v>4394</v>
+      </c>
+      <c r="E741" s="1" t="s">
+        <v>4395</v>
+      </c>
+      <c r="F741" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="G741" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="H741" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="I741" s="0" t="s">
+        <v>4301</v>
+      </c>
+      <c r="J741" s="0" t="s">
+        <v>4302</v>
+      </c>
+      <c r="K741" s="0" t="s">
+        <v>4013</v>
+      </c>
+    </row>
+    <row r="742" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A742" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B742" s="0" t="s">
+        <v>4396</v>
+      </c>
+      <c r="C742" s="0" t="s">
+        <v>4396</v>
+      </c>
+      <c r="D742" s="0" t="s">
+        <v>4397</v>
+      </c>
+      <c r="E742" s="0" t="s">
+        <v>4398</v>
+      </c>
+      <c r="F742" s="0" t="s">
+        <v>1029</v>
+      </c>
+      <c r="G742" s="0" t="s">
+        <v>4399</v>
+      </c>
+      <c r="H742" s="0" t="s">
+        <v>4400</v>
+      </c>
+      <c r="I742" s="0" t="s">
+        <v>4401</v>
+      </c>
+      <c r="J742" s="0" t="s">
+        <v>4402</v>
+      </c>
+      <c r="K742" s="0" t="s">
+        <v>3653</v>
+      </c>
+    </row>
+    <row r="743" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A743" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B743" s="0" t="s">
+        <v>4403</v>
+      </c>
+      <c r="C743" s="0" t="s">
+        <v>4403</v>
+      </c>
+      <c r="D743" s="0" t="s">
+        <v>4404</v>
+      </c>
+      <c r="E743" s="1" t="s">
+        <v>4405</v>
+      </c>
+      <c r="F743" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="G743" s="0" t="s">
+        <v>4316</v>
+      </c>
+      <c r="H743" s="0" t="s">
+        <v>609</v>
+      </c>
+      <c r="I743" s="0" t="s">
+        <v>4406</v>
+      </c>
+      <c r="J743" s="0" t="s">
+        <v>4407</v>
+      </c>
+      <c r="K743" s="0" t="s">
+        <v>3653</v>
+      </c>
+    </row>
+    <row r="744" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A744" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B744" s="0" t="s">
+        <v>4408</v>
+      </c>
+      <c r="C744" s="0" t="s">
+        <v>4408</v>
+      </c>
+      <c r="D744" s="0" t="s">
+        <v>4409</v>
+      </c>
+      <c r="E744" s="0" t="s">
+        <v>4410</v>
+      </c>
+      <c r="F744" s="0" t="s">
+        <v>4411</v>
+      </c>
+      <c r="G744" s="0" t="s">
+        <v>4265</v>
+      </c>
+      <c r="H744" s="0" t="s">
+        <v>2214</v>
+      </c>
+      <c r="I744" s="0" t="s">
+        <v>4412</v>
+      </c>
+      <c r="J744" s="0" t="s">
+        <v>4413</v>
+      </c>
+      <c r="K744" s="0" t="s">
+        <v>3653</v>
+      </c>
+    </row>
+    <row r="745" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A745" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B745" s="0" t="s">
+        <v>4414</v>
+      </c>
+      <c r="C745" s="0" t="s">
+        <v>4414</v>
+      </c>
+      <c r="D745" s="0" t="s">
+        <v>4415</v>
+      </c>
+      <c r="E745" s="0" t="s">
+        <v>2804</v>
+      </c>
+      <c r="F745" s="0" t="s">
+        <v>2805</v>
+      </c>
+      <c r="G745" s="0" t="s">
+        <v>4258</v>
+      </c>
+      <c r="H745" s="0" t="s">
+        <v>4293</v>
+      </c>
+      <c r="I745" s="0" t="s">
+        <v>4416</v>
+      </c>
+      <c r="J745" s="0" t="s">
+        <v>4417</v>
+      </c>
+      <c r="K745" s="0" t="s">
+        <v>3949</v>
+      </c>
+    </row>
+    <row r="746" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A746" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B746" s="0" t="s">
+        <v>4418</v>
+      </c>
+      <c r="C746" s="0" t="s">
+        <v>4419</v>
+      </c>
+      <c r="D746" s="0" t="s">
+        <v>4420</v>
+      </c>
+      <c r="E746" s="0" t="s">
+        <v>4421</v>
+      </c>
+      <c r="F746" s="0" t="s">
+        <v>4422</v>
+      </c>
+      <c r="G746" s="0" t="s">
+        <v>4285</v>
+      </c>
+      <c r="H746" s="0" t="s">
+        <v>2151</v>
+      </c>
+      <c r="I746" s="0" t="s">
+        <v>4207</v>
+      </c>
+      <c r="J746" s="0" t="s">
+        <v>4208</v>
+      </c>
+      <c r="K746" s="0" t="s">
+        <v>3949</v>
+      </c>
+    </row>
+    <row r="747" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A747" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B747" s="0" t="s">
+        <v>4423</v>
+      </c>
+      <c r="C747" s="0" t="s">
+        <v>4424</v>
+      </c>
+      <c r="D747" s="0" t="s">
+        <v>4425</v>
+      </c>
+      <c r="E747" s="0" t="s">
+        <v>4426</v>
+      </c>
+      <c r="F747" s="0" t="s">
+        <v>4427</v>
+      </c>
+      <c r="G747" s="0" t="s">
+        <v>4275</v>
+      </c>
+      <c r="H747" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="I747" s="0" t="s">
+        <v>4428</v>
+      </c>
+      <c r="J747" s="0" t="s">
+        <v>4429</v>
+      </c>
+      <c r="K747" s="0" t="s">
+        <v>3489</v>
+      </c>
+      <c r="L747" s="0" t="s">
+        <v>4430</v>
+      </c>
+    </row>
+    <row r="748" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A748" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B748" s="0" t="s">
+        <v>4431</v>
+      </c>
+      <c r="C748" s="0" t="s">
+        <v>4432</v>
+      </c>
+      <c r="D748" s="0" t="s">
+        <v>4433</v>
+      </c>
+      <c r="E748" s="0" t="s">
+        <v>4421</v>
+      </c>
+      <c r="F748" s="0" t="s">
+        <v>4422</v>
+      </c>
+      <c r="G748" s="0" t="s">
+        <v>4285</v>
+      </c>
+      <c r="H748" s="0" t="s">
+        <v>1296</v>
+      </c>
+      <c r="I748" s="0" t="s">
+        <v>4039</v>
+      </c>
+      <c r="J748" s="0" t="s">
+        <v>4040</v>
+      </c>
+      <c r="K748" s="0" t="s">
+        <v>3992</v>
+      </c>
+    </row>
+    <row r="749" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A749" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B749" s="0" t="s">
+        <v>4434</v>
+      </c>
+      <c r="C749" s="0" t="s">
+        <v>4434</v>
+      </c>
+      <c r="D749" s="0" t="s">
+        <v>4435</v>
+      </c>
+      <c r="E749" s="0" t="s">
+        <v>4436</v>
+      </c>
+      <c r="F749" s="0" t="s">
+        <v>4437</v>
+      </c>
+      <c r="G749" s="0" t="s">
+        <v>4383</v>
+      </c>
+      <c r="H749" s="0" t="s">
+        <v>1296</v>
+      </c>
+      <c r="I749" s="0" t="s">
+        <v>4438</v>
+      </c>
+      <c r="K749" s="0" t="s">
+        <v>3958</v>
+      </c>
+    </row>
+    <row r="750" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A750" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B750" s="0" t="s">
+        <v>4439</v>
+      </c>
+      <c r="C750" s="0" t="s">
+        <v>4440</v>
+      </c>
+      <c r="D750" s="0" t="s">
+        <v>4441</v>
+      </c>
+      <c r="E750" s="0" t="s">
+        <v>4439</v>
+      </c>
+      <c r="F750" s="0" t="s">
+        <v>4442</v>
+      </c>
+      <c r="G750" s="0" t="s">
+        <v>4275</v>
+      </c>
+      <c r="H750" s="0" t="s">
+        <v>911</v>
+      </c>
+      <c r="I750" s="0" t="s">
+        <v>4443</v>
+      </c>
+      <c r="J750" s="0" t="s">
+        <v>4444</v>
+      </c>
+      <c r="K750" s="0" t="s">
+        <v>3992</v>
+      </c>
+    </row>
+    <row r="751" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A751" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B751" s="0" t="s">
+        <v>4445</v>
+      </c>
+      <c r="C751" s="0" t="s">
+        <v>4445</v>
+      </c>
+      <c r="D751" s="0" t="s">
+        <v>4446</v>
+      </c>
+      <c r="E751" s="0" t="s">
+        <v>2804</v>
+      </c>
+      <c r="F751" s="0" t="s">
+        <v>2805</v>
+      </c>
+      <c r="G751" s="0" t="s">
+        <v>4265</v>
+      </c>
+      <c r="H751" s="0" t="s">
+        <v>4447</v>
+      </c>
+      <c r="I751" s="0" t="s">
+        <v>4448</v>
+      </c>
+      <c r="J751" s="0" t="s">
+        <v>4449</v>
+      </c>
+      <c r="K751" s="0" t="s">
+        <v>3653</v>
+      </c>
+    </row>
+    <row r="752" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A752" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B752" s="0" t="s">
+        <v>4450</v>
+      </c>
+      <c r="C752" s="0" t="s">
+        <v>4451</v>
+      </c>
+      <c r="D752" s="0" t="s">
+        <v>4452</v>
+      </c>
+      <c r="E752" s="0" t="s">
+        <v>4453</v>
+      </c>
+      <c r="F752" s="0" t="s">
+        <v>4454</v>
+      </c>
+      <c r="G752" s="0" t="s">
+        <v>4455</v>
+      </c>
+      <c r="H752" s="0" t="s">
+        <v>555</v>
+      </c>
+      <c r="I752" s="0" t="s">
+        <v>3956</v>
+      </c>
+      <c r="J752" s="0" t="s">
+        <v>3957</v>
+      </c>
+      <c r="K752" s="0" t="s">
+        <v>3958</v>
+      </c>
+    </row>
+    <row r="753" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A753" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B753" s="0" t="s">
+        <v>4456</v>
+      </c>
+      <c r="C753" s="0" t="s">
+        <v>4457</v>
+      </c>
+      <c r="D753" s="0" t="s">
+        <v>4458</v>
+      </c>
+      <c r="E753" s="0" t="s">
+        <v>989</v>
+      </c>
+      <c r="F753" s="0" t="s">
+        <v>990</v>
+      </c>
+      <c r="G753" s="0" t="s">
+        <v>4316</v>
+      </c>
+      <c r="H753" s="0" t="s">
+        <v>609</v>
+      </c>
+      <c r="I753" s="0" t="s">
+        <v>4072</v>
+      </c>
+      <c r="J753" s="0" t="s">
+        <v>4073</v>
+      </c>
+      <c r="K753" s="0" t="s">
+        <v>3992</v>
+      </c>
+    </row>
+    <row r="754" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A754" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B754" s="0" t="s">
+        <v>4459</v>
+      </c>
+      <c r="C754" s="0" t="s">
+        <v>4460</v>
+      </c>
+      <c r="D754" s="0" t="s">
+        <v>4461</v>
+      </c>
+      <c r="E754" s="0" t="s">
+        <v>4462</v>
+      </c>
+      <c r="F754" s="0" t="s">
+        <v>1319</v>
+      </c>
+      <c r="G754" s="0" t="s">
+        <v>4383</v>
+      </c>
+      <c r="H754" s="0" t="s">
+        <v>1296</v>
+      </c>
+      <c r="I754" s="0" t="s">
+        <v>3990</v>
+      </c>
+      <c r="J754" s="0" t="s">
+        <v>3991</v>
+      </c>
+      <c r="K754" s="0" t="s">
+        <v>3992</v>
+      </c>
+    </row>
+    <row r="755" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A755" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B755" s="0" t="s">
+        <v>4463</v>
+      </c>
+      <c r="C755" s="0" t="s">
+        <v>4464</v>
+      </c>
+      <c r="D755" s="0" t="s">
+        <v>4465</v>
+      </c>
+      <c r="E755" s="0" t="s">
+        <v>3367</v>
+      </c>
+      <c r="F755" s="0" t="s">
+        <v>3368</v>
+      </c>
+      <c r="G755" s="0" t="s">
+        <v>4285</v>
+      </c>
+      <c r="H755" s="0" t="s">
+        <v>1296</v>
+      </c>
+      <c r="I755" s="0" t="s">
+        <v>4142</v>
+      </c>
+      <c r="J755" s="0" t="s">
+        <v>4143</v>
+      </c>
+      <c r="K755" s="0" t="s">
+        <v>3949</v>
+      </c>
+    </row>
+    <row r="756" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A756" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B756" s="0" t="s">
+        <v>4466</v>
+      </c>
+      <c r="C756" s="0" t="s">
+        <v>4467</v>
+      </c>
+      <c r="D756" s="0" t="s">
+        <v>829</v>
+      </c>
+      <c r="E756" s="0" t="s">
+        <v>4468</v>
+      </c>
+      <c r="F756" s="0" t="s">
+        <v>4469</v>
+      </c>
+      <c r="G756" s="0" t="s">
+        <v>4316</v>
+      </c>
+      <c r="H756" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="I756" s="0" t="s">
+        <v>4470</v>
+      </c>
+      <c r="J756" s="0" t="s">
+        <v>4471</v>
+      </c>
+      <c r="K756" s="0" t="s">
+        <v>4013</v>
+      </c>
+    </row>
+    <row r="757" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A757" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B757" s="0" t="s">
+        <v>4472</v>
+      </c>
+      <c r="C757" s="0" t="s">
+        <v>3373</v>
+      </c>
+      <c r="D757" s="0" t="s">
+        <v>3374</v>
+      </c>
+      <c r="E757" s="0" t="s">
+        <v>3375</v>
+      </c>
+      <c r="F757" s="0" t="s">
+        <v>3376</v>
+      </c>
+      <c r="G757" s="0" t="s">
+        <v>4316</v>
+      </c>
+      <c r="H757" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="I757" s="0" t="s">
+        <v>4473</v>
+      </c>
+      <c r="J757" s="0" t="s">
+        <v>4474</v>
+      </c>
+      <c r="K757" s="0" t="s">
+        <v>3489</v>
+      </c>
+    </row>
+    <row r="758" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A758" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B758" s="0" t="s">
+        <v>4475</v>
+      </c>
+      <c r="C758" s="0" t="s">
+        <v>4475</v>
+      </c>
+      <c r="D758" s="0" t="s">
+        <v>4476</v>
+      </c>
+      <c r="E758" s="0" t="s">
+        <v>4477</v>
+      </c>
+      <c r="F758" s="0" t="s">
+        <v>4478</v>
+      </c>
+      <c r="G758" s="0" t="s">
+        <v>4275</v>
+      </c>
+      <c r="H758" s="0" t="s">
+        <v>609</v>
+      </c>
+      <c r="I758" s="0" t="s">
+        <v>4479</v>
+      </c>
+      <c r="J758" s="0" t="s">
+        <v>4480</v>
+      </c>
+      <c r="K758" s="0" t="s">
+        <v>4013</v>
+      </c>
+    </row>
+    <row r="759" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A759" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B759" s="0" t="s">
+        <v>4481</v>
+      </c>
+      <c r="C759" s="0" t="s">
+        <v>2880</v>
+      </c>
+      <c r="D759" s="0" t="s">
+        <v>2881</v>
+      </c>
+      <c r="E759" s="0" t="s">
+        <v>1007</v>
+      </c>
+      <c r="F759" s="0" t="s">
+        <v>1008</v>
+      </c>
+      <c r="G759" s="0" t="s">
+        <v>4316</v>
+      </c>
+      <c r="H759" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="I759" s="0" t="s">
+        <v>4072</v>
+      </c>
+      <c r="J759" s="0" t="s">
+        <v>4073</v>
+      </c>
+      <c r="K759" s="0" t="s">
+        <v>3992</v>
+      </c>
+    </row>
+    <row r="760" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A760" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B760" s="0" t="s">
+        <v>4482</v>
+      </c>
+      <c r="C760" s="0" t="s">
+        <v>4483</v>
+      </c>
+      <c r="D760" s="0" t="s">
+        <v>4321</v>
+      </c>
+      <c r="E760" s="0" t="s">
+        <v>4484</v>
+      </c>
+      <c r="F760" s="0" t="s">
+        <v>4323</v>
+      </c>
+      <c r="G760" s="0" t="s">
+        <v>4285</v>
+      </c>
+      <c r="H760" s="0" t="s">
+        <v>2151</v>
+      </c>
+      <c r="I760" s="0" t="s">
+        <v>4097</v>
+      </c>
+      <c r="J760" s="0" t="s">
+        <v>4098</v>
+      </c>
+      <c r="K760" s="0" t="s">
+        <v>3489</v>
+      </c>
+    </row>
+    <row r="761" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A761" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B761" s="0" t="s">
+        <v>4485</v>
+      </c>
+      <c r="C761" s="0" t="s">
+        <v>4486</v>
+      </c>
+      <c r="D761" s="0" t="s">
+        <v>4487</v>
+      </c>
+      <c r="E761" s="0" t="s">
+        <v>3389</v>
+      </c>
+      <c r="F761" s="0" t="s">
+        <v>4488</v>
+      </c>
+      <c r="G761" s="0" t="s">
+        <v>4258</v>
+      </c>
+      <c r="H761" s="0" t="s">
+        <v>2801</v>
+      </c>
+      <c r="I761" s="0" t="s">
+        <v>4200</v>
+      </c>
+      <c r="J761" s="0" t="s">
+        <v>4201</v>
+      </c>
+      <c r="K761" s="0" t="s">
+        <v>3992</v>
+      </c>
+    </row>
+    <row r="762" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A762" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B762" s="0" t="s">
+        <v>4489</v>
+      </c>
+      <c r="C762" s="0" t="s">
+        <v>2285</v>
+      </c>
+      <c r="D762" s="0" t="s">
+        <v>2286</v>
+      </c>
+      <c r="E762" s="0" t="s">
+        <v>4490</v>
+      </c>
+      <c r="F762" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="G762" s="0" t="s">
+        <v>4491</v>
+      </c>
+      <c r="H762" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="I762" s="0" t="s">
+        <v>4492</v>
+      </c>
+      <c r="J762" s="0" t="s">
+        <v>4493</v>
+      </c>
+      <c r="K762" s="0" t="s">
+        <v>3653</v>
+      </c>
+      <c r="L762" s="0" t="s">
+        <v>2291</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Generated files, and more added xg, compg andcontlex values.
git-svn-id: https://gtsvn.uit.no/langtech/trunk/langs/sms@152878 c7155fb1-f0a7-4240-a2fc-2600b6f42f90
</commit_message>
<xml_diff>
--- a/src/morphology/incoming/Compg_sms.xlsx
+++ b/src/morphology/incoming/Compg_sms.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9084" uniqueCount="5139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9390" uniqueCount="5321">
   <si>
     <t xml:space="preserve">Tyyppi</t>
   </si>
@@ -15608,6 +15608,552 @@
   </si>
   <si>
     <t xml:space="preserve">Talvikaivinpaikoissa niin kaivavat. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">17.5.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">auttkoloonn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">auttkolonn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">autokolonna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">autt+kolonn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">auto+kolonna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peäccmest nuʹtt puäʹđškuõʹtte auttkoloonn.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Petsamossa rupesi tulemaan autokolonnoita.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VJO s. 90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jeällsââi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nâ ij kâʹl tõn še jeällsââi vueiʹt ǩeiʹtted.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eipä kyllä sitäkään asuinpaikkaa voi kehua. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VJO s. 91</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ǩeʹddpååʹštaautin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ǩeʹddpååʹštautt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kenttäpostiauto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ǩeʹddpååʹšt+autt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kenttäposti+auto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Âʹvvlest kuäʹss ku jieʹlim kaaupâst ǩeässa, tâʹl jieʹlim Lååttčuõkku mieʹldd ǩeʹddpååʹštaautin.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kun kävimme Ivalossa kaupassa kesällä, silloin menimme Lutontietä kenttäpostiautolla. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ǩeʹttemsââʹjjen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ǩeʹttemsââʹjj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">keittopaikka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ǩeʹttem+sââʹjj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">keittäminen+paikka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V(akt)+N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ǩeʹttemsââʹjjen leäi õhtt ruʹvddǩiuggân.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keittopaikkana oli yksi hella. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ǩeäzzõkeeʹǩǩ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lauha vuosi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ǩeäzzõk+eeʹǩǩ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kesäinen ilma+vuosi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tâʹl leäi kuʹǩes ǩeäzzõkeeʹǩǩ, rosttovmannust veâl iʹlleämma muõtt, sami rosttvid eman kuâldai.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sinä vuonna oli pitkään lämpimät ilmat, vielä joulukuussakaan ei ollut lunta, vasta jouluna satoi lumi. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ǩieʹsspõrtt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kesäasunto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ǩieʹss+põrtt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kesä+talo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tâʹl mij mõõnim Ceeʒʒanjaʹrǧǧe. Toʹben leäi måttmin oummin ǩieʹsspõrtt, jõnn šiõǥǥ põrtt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sitten menimme Tiaisniemeen. Siellä oli muutamilla ihmisillä kesäasunto, iso hyvä talo. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kueʹddemkõskk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kantoväli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kueʹddem+kõskk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kantaminen+väli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tõiʹnn leäi hiâlpab jieʹlled, kueʹddemkõskk šõõddi vuäʹnkab.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sillä oli helpompi kulkea, kantovälistä tuli lyhempi. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">nuõrrseäʹbrrpõʹrtte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nuõrrseäʹbrrpõrtt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nuorisoseurantalo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nuõrrseäʹbrr+põrtt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nuorisoseura+talo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rahja siid nuõrrseäʹbrrpõʹrtte piâzzim sizz.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rahjan kylän nuorisoseurantalolle pääsimme sisään. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">obbmieʹlǩ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">obbmieʹlǩǩ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">täysmaito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">obb+mieʹlǩǩ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kokonainen+maito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Väinnääiʹj ij vuäǯǯam ni vooʹps obbmieʹlǩ di jiâ ni jiijj koiʹnn leʹjje kuuzz.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sota-aikana ei saanut ollenkaan täysmaitoa, eivät edes ne, joilla itsellään oli lehmiä. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rosttovmannust</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rosttovmään</t>
+  </si>
+  <si>
+    <t xml:space="preserve">joulukuu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rosttov+mään</t>
+  </si>
+  <si>
+    <t xml:space="preserve">joulu+kuu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ruʹvddčuõkku</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ruʹvddčuâǥǥas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rautatie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ruʹvdd+čuâǥǥâs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rauta+tie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ruäʹvnjaarǥâst ooudâs vuõʹljiim ruʹvddčuõkku mieʹldd.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rovaniemeltä eteenpäin lähdimme rautatietä pitkin. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ruʹvddǩiuggân</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ruʹvdd+ǩiuggân</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rauta+uuni</t>
+  </si>
+  <si>
+    <t xml:space="preserve">täʹǩǩpõõrtâst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">täʹǩǩpõrtt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">takkahuone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">täʹǩǩ+põrtt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">takka+talo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jiijj vuäʹđđe päärneezvuiʹm kämmrest, mij-ǥõs täʹǩǩpõõrtâst.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Itse nukkuvat lapsineen kamarissa, me taas takkahuoneessa. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">täʹvverjunavaaunin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">täʹvverjunavaunn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tavarajunavaunu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">täʹvverjuna+vaunn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tavarajuna+vaunu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Täʹvverjunavaaunin leeiʹm puk oummu še.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tavarjunavaunuissa olimme myös kaikki ihmiset. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">vuäʹmmpäʹrnn da -nijdd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vanhapoika ja -piika</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vuäʹmm+päʹrnn, (vuäʹmm)+nijdd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vanha+poika, (vanha)+tyttö</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toʹben leʹjje källaz villj da vuäʹbb, vuäʹmmpäʹrnn da -nijdd.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Siellä olivat ukon veli ja sisko, vanhapoika ja -piika. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">cõõjõõđad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cõõjõõđeed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">siirtyillä</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cõõjõõttâd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">siirtyä</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V»V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juna tõt oudsmååust cõõjõõđad, pâi špooukâs da škall mâânn.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juna se siirtyilee edestakaisin, vain pauke ja kolina kuuluu. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">čuõʒʒtõõđi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">čuõʒʒtõõttâd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">loukkaantua (fyysisesti)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">čueʹcced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sattua</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Der/tõõttâd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Son leäi vueʹrddmen mââimõs mannust, kaaggi mõõn leežž loʹsses čââʹǧǧ, tõʹst čuõʒʒtõõđi.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hän oli raskaana viimeisellä kuulla, nosti jotakin raskasta taakkaa ja siinä loukkasi itsensä. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">jååʹđteškuõʹđi </t>
+  </si>
+  <si>
+    <t xml:space="preserve">soveltua kuljettavaksi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ǩieʹssmään leäi juʹn peäʹlrääʹjest, ku Aanar jååʹđteškuõʹđi moto­rin. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kesäkuu oli jo puolessa välissä, kun Inarinjärvellä pystyi taas liikkumaan moottoriveneellä (sananmukaisesti: kun Inari kuljetti moottorilla). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kuâldai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kuâldd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lumisade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N»V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kååškõk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kuiva ilma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kååʹšǩes # kåʹšǩǩ-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A»N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Čõhčč veâl leäi, de ålggan jeänaš ǩiiʹttim, ku leäi kååškõk.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oli vielä syksy, ja keitimme enimmäkseen ulkona, koska oli kuiva ilma. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">meärrõs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">määräys</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V»N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1944 ǩiđđmannust pueʹđi meärrõs: âlgg Njeäʹllma seʹrdded.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toukokuussa 1944 tuli määräys: pitää muuttaa Nellimiin. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">miâttčõõđim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">miâttčõõttâd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pakata tavaransa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*miâttčed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pakkailla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teä mij pâi eʹpet miâttčõõđim.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sitten vain taas pakkasimme tavaramme. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">miâttčed &lt; meäʹtted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">muõtt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lumi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*mueʹtted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Der/âǥ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">paʹǩǩõõđim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">paʹǩǩõõttâd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">paʹǩǩeed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pakata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tõʹst paʹǩǩõõđim muäʹdd peiʹvved.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Siellä pakkasimme tavaroitamme muutaman päivän. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">põõltõs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pelottava</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V»A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Der/tõs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Čâhčča ku liâ kuʹǩes seuʹŋŋes jeäʹǩǩää, måtam vuâra lij nuʹtt põõltõs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kun syksyllä on pitkät synkät illat, toinsinaan on niin pelottavaa. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">seeʹrdte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">seeʹrdted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">siirtää</t>
+  </si>
+  <si>
+    <t xml:space="preserve">seʹrdded</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tõʹst âʹte miʹjjid seeʹrdte motorivuiʹm Njeäʹllma.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Siitä meidät siirrettiin moottoriveneillä Nellimiin. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">taʹrǩǩeeja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tarkastaja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">taʹrǩǩeed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tarkistaa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juõʹǩǩ mannust jooʹđi tõt taʹrǩǩeeja, mâʹmmet kuuzz pâʹčča mieʹlǩ da mâʹmmet vuõjjân šâdd.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joka kuussa kulki se tarkastaja, paljonko lehmät lypsävät ja paljonko tulee voiksi.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VJO s. 92</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tuõʹlddstâʹtted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kiehauttaa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tuõʹlddsted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kiehahtaa (vähän)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mij leeiʹm vittmlo piârrjed, kååʹtt kuäʹss ǩirggan čeeiʹnǩes da ǩieʹmnes tuõʹlddstâʹtted.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meitä oli viisitoista perhettä, kuka milloinkin ehtii kiehauttaa teepannunsa ja kattilansa. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ääkkiʹʒʒin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ääkkiʹʒʒe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mummon perhe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">äkk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mummo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N»N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Der/iʹʒʒe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ääkkiʹʒʒin Uʹlljnaž jaaʹmi.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mummon perheessä Uljaana kuoli. </t>
   </si>
 </sst>
 </file>
@@ -15773,26 +16319,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L878"/>
+  <dimension ref="A1:L909"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A810" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B817" activeCellId="0" sqref="B817"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A874" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A879" activeCellId="0" sqref="A879"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.66326530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.8520408163265"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.1938775510204"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.8520408163265"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.5357142857143"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.1020408163265"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.530612244898"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="30.4642857142857"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="27.6173469387755"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.66326530612245"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="19.780612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="9.66326530612245"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.4438775510204"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.7857142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.4438775510204"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.1275510204082"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.1479591836735"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.780612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="32.5051020408163"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="29.5561224489796"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.3469387755102"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.1377551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="10.3469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44763,6 +45309,984 @@
       </c>
       <c r="J878" s="0" t="s">
         <v>5138</v>
+      </c>
+    </row>
+    <row r="880" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A880" s="4" t="s">
+        <v>5139</v>
+      </c>
+      <c r="B880" s="0" t="s">
+        <v>5139</v>
+      </c>
+    </row>
+    <row r="881" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A881" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B881" s="0" t="s">
+        <v>5140</v>
+      </c>
+      <c r="C881" s="0" t="s">
+        <v>5141</v>
+      </c>
+      <c r="D881" s="0" t="s">
+        <v>5142</v>
+      </c>
+      <c r="E881" s="0" t="s">
+        <v>5143</v>
+      </c>
+      <c r="F881" s="0" t="s">
+        <v>5144</v>
+      </c>
+      <c r="G881" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I881" s="0" t="s">
+        <v>5145</v>
+      </c>
+      <c r="J881" s="0" t="s">
+        <v>5146</v>
+      </c>
+      <c r="K881" s="0" t="s">
+        <v>5147</v>
+      </c>
+    </row>
+    <row r="882" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A882" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B882" s="0" t="s">
+        <v>5148</v>
+      </c>
+      <c r="C882" s="0" t="s">
+        <v>3508</v>
+      </c>
+      <c r="D882" s="0" t="s">
+        <v>3509</v>
+      </c>
+      <c r="E882" s="0" t="s">
+        <v>3510</v>
+      </c>
+      <c r="F882" s="0" t="s">
+        <v>3511</v>
+      </c>
+      <c r="G882" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I882" s="0" t="s">
+        <v>5149</v>
+      </c>
+      <c r="J882" s="0" t="s">
+        <v>5150</v>
+      </c>
+      <c r="K882" s="0" t="s">
+        <v>5151</v>
+      </c>
+    </row>
+    <row r="883" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A883" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B883" s="0" t="s">
+        <v>5152</v>
+      </c>
+      <c r="C883" s="0" t="s">
+        <v>5153</v>
+      </c>
+      <c r="D883" s="0" t="s">
+        <v>5154</v>
+      </c>
+      <c r="E883" s="0" t="s">
+        <v>5155</v>
+      </c>
+      <c r="F883" s="0" t="s">
+        <v>5156</v>
+      </c>
+      <c r="G883" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I883" s="0" t="s">
+        <v>5157</v>
+      </c>
+      <c r="J883" s="0" t="s">
+        <v>5158</v>
+      </c>
+      <c r="K883" s="0" t="s">
+        <v>5147</v>
+      </c>
+    </row>
+    <row r="884" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A884" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B884" s="0" t="s">
+        <v>5159</v>
+      </c>
+      <c r="C884" s="0" t="s">
+        <v>5160</v>
+      </c>
+      <c r="D884" s="0" t="s">
+        <v>5161</v>
+      </c>
+      <c r="E884" s="0" t="s">
+        <v>5162</v>
+      </c>
+      <c r="F884" s="0" t="s">
+        <v>5163</v>
+      </c>
+      <c r="G884" s="0" t="s">
+        <v>5164</v>
+      </c>
+      <c r="I884" s="0" t="s">
+        <v>5165</v>
+      </c>
+      <c r="J884" s="0" t="s">
+        <v>5166</v>
+      </c>
+      <c r="K884" s="0" t="s">
+        <v>5151</v>
+      </c>
+    </row>
+    <row r="885" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A885" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B885" s="0" t="s">
+        <v>5167</v>
+      </c>
+      <c r="C885" s="0" t="s">
+        <v>5167</v>
+      </c>
+      <c r="D885" s="0" t="s">
+        <v>5168</v>
+      </c>
+      <c r="E885" s="0" t="s">
+        <v>5169</v>
+      </c>
+      <c r="F885" s="0" t="s">
+        <v>5170</v>
+      </c>
+      <c r="G885" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I885" s="0" t="s">
+        <v>5171</v>
+      </c>
+      <c r="J885" s="0" t="s">
+        <v>5172</v>
+      </c>
+      <c r="K885" s="0" t="s">
+        <v>5151</v>
+      </c>
+    </row>
+    <row r="886" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A886" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B886" s="0" t="s">
+        <v>5173</v>
+      </c>
+      <c r="C886" s="0" t="s">
+        <v>5173</v>
+      </c>
+      <c r="D886" s="0" t="s">
+        <v>5174</v>
+      </c>
+      <c r="E886" s="0" t="s">
+        <v>5175</v>
+      </c>
+      <c r="F886" s="0" t="s">
+        <v>5176</v>
+      </c>
+      <c r="G886" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I886" s="0" t="s">
+        <v>5177</v>
+      </c>
+      <c r="J886" s="0" t="s">
+        <v>5178</v>
+      </c>
+      <c r="K886" s="0" t="s">
+        <v>5147</v>
+      </c>
+    </row>
+    <row r="887" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A887" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B887" s="0" t="s">
+        <v>5179</v>
+      </c>
+      <c r="C887" s="0" t="s">
+        <v>5179</v>
+      </c>
+      <c r="D887" s="0" t="s">
+        <v>5180</v>
+      </c>
+      <c r="E887" s="0" t="s">
+        <v>5181</v>
+      </c>
+      <c r="F887" s="0" t="s">
+        <v>5182</v>
+      </c>
+      <c r="G887" s="0" t="s">
+        <v>5164</v>
+      </c>
+      <c r="I887" s="0" t="s">
+        <v>5183</v>
+      </c>
+      <c r="J887" s="0" t="s">
+        <v>5184</v>
+      </c>
+      <c r="K887" s="0" t="s">
+        <v>5147</v>
+      </c>
+    </row>
+    <row r="888" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A888" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B888" s="0" t="s">
+        <v>5185</v>
+      </c>
+      <c r="C888" s="0" t="s">
+        <v>5186</v>
+      </c>
+      <c r="D888" s="0" t="s">
+        <v>5187</v>
+      </c>
+      <c r="E888" s="0" t="s">
+        <v>5188</v>
+      </c>
+      <c r="F888" s="0" t="s">
+        <v>5189</v>
+      </c>
+      <c r="G888" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I888" s="0" t="s">
+        <v>5190</v>
+      </c>
+      <c r="J888" s="0" t="s">
+        <v>5191</v>
+      </c>
+      <c r="K888" s="0" t="s">
+        <v>5151</v>
+      </c>
+    </row>
+    <row r="889" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A889" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B889" s="0" t="s">
+        <v>5192</v>
+      </c>
+      <c r="C889" s="0" t="s">
+        <v>5193</v>
+      </c>
+      <c r="D889" s="0" t="s">
+        <v>5194</v>
+      </c>
+      <c r="E889" s="0" t="s">
+        <v>5195</v>
+      </c>
+      <c r="F889" s="0" t="s">
+        <v>5196</v>
+      </c>
+      <c r="G889" s="0" t="s">
+        <v>4644</v>
+      </c>
+      <c r="I889" s="0" t="s">
+        <v>5197</v>
+      </c>
+      <c r="J889" s="0" t="s">
+        <v>5198</v>
+      </c>
+      <c r="K889" s="0" t="s">
+        <v>5151</v>
+      </c>
+    </row>
+    <row r="890" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A890" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B890" s="0" t="s">
+        <v>5199</v>
+      </c>
+      <c r="C890" s="0" t="s">
+        <v>5200</v>
+      </c>
+      <c r="D890" s="0" t="s">
+        <v>5201</v>
+      </c>
+      <c r="E890" s="0" t="s">
+        <v>5202</v>
+      </c>
+      <c r="F890" s="0" t="s">
+        <v>5203</v>
+      </c>
+      <c r="G890" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I890" s="0" t="s">
+        <v>5171</v>
+      </c>
+      <c r="J890" s="0" t="s">
+        <v>5172</v>
+      </c>
+      <c r="K890" s="0" t="s">
+        <v>5151</v>
+      </c>
+    </row>
+    <row r="891" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A891" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B891" s="0" t="s">
+        <v>5204</v>
+      </c>
+      <c r="C891" s="0" t="s">
+        <v>5205</v>
+      </c>
+      <c r="D891" s="0" t="s">
+        <v>5206</v>
+      </c>
+      <c r="E891" s="0" t="s">
+        <v>5207</v>
+      </c>
+      <c r="F891" s="0" t="s">
+        <v>5208</v>
+      </c>
+      <c r="G891" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I891" s="0" t="s">
+        <v>5209</v>
+      </c>
+      <c r="J891" s="0" t="s">
+        <v>5210</v>
+      </c>
+      <c r="K891" s="0" t="s">
+        <v>5147</v>
+      </c>
+    </row>
+    <row r="892" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A892" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B892" s="0" t="s">
+        <v>5211</v>
+      </c>
+      <c r="C892" s="0" t="s">
+        <v>5211</v>
+      </c>
+      <c r="D892" s="0" t="s">
+        <v>4904</v>
+      </c>
+      <c r="E892" s="0" t="s">
+        <v>5212</v>
+      </c>
+      <c r="F892" s="0" t="s">
+        <v>5213</v>
+      </c>
+      <c r="G892" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I892" s="0" t="s">
+        <v>5165</v>
+      </c>
+      <c r="J892" s="0" t="s">
+        <v>5166</v>
+      </c>
+      <c r="K892" s="0" t="s">
+        <v>5151</v>
+      </c>
+    </row>
+    <row r="893" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A893" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B893" s="0" t="s">
+        <v>5214</v>
+      </c>
+      <c r="C893" s="0" t="s">
+        <v>5215</v>
+      </c>
+      <c r="D893" s="0" t="s">
+        <v>5216</v>
+      </c>
+      <c r="E893" s="0" t="s">
+        <v>5217</v>
+      </c>
+      <c r="F893" s="0" t="s">
+        <v>5218</v>
+      </c>
+      <c r="G893" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I893" s="0" t="s">
+        <v>5219</v>
+      </c>
+      <c r="J893" s="0" t="s">
+        <v>5220</v>
+      </c>
+      <c r="K893" s="0" t="s">
+        <v>5151</v>
+      </c>
+    </row>
+    <row r="894" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A894" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B894" s="0" t="s">
+        <v>5221</v>
+      </c>
+      <c r="C894" s="0" t="s">
+        <v>5222</v>
+      </c>
+      <c r="D894" s="0" t="s">
+        <v>5223</v>
+      </c>
+      <c r="E894" s="0" t="s">
+        <v>5224</v>
+      </c>
+      <c r="F894" s="0" t="s">
+        <v>5225</v>
+      </c>
+      <c r="G894" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I894" s="0" t="s">
+        <v>5226</v>
+      </c>
+      <c r="J894" s="0" t="s">
+        <v>5227</v>
+      </c>
+      <c r="K894" s="0" t="s">
+        <v>5147</v>
+      </c>
+    </row>
+    <row r="895" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A895" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B895" s="0" t="s">
+        <v>5228</v>
+      </c>
+      <c r="C895" s="0" t="s">
+        <v>5228</v>
+      </c>
+      <c r="D895" s="0" t="s">
+        <v>5229</v>
+      </c>
+      <c r="E895" s="0" t="s">
+        <v>5230</v>
+      </c>
+      <c r="F895" s="0" t="s">
+        <v>5231</v>
+      </c>
+      <c r="G895" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I895" s="0" t="s">
+        <v>5232</v>
+      </c>
+      <c r="J895" s="0" t="s">
+        <v>5233</v>
+      </c>
+      <c r="K895" s="0" t="s">
+        <v>5151</v>
+      </c>
+    </row>
+    <row r="896" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A896" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B896" s="0" t="s">
+        <v>5234</v>
+      </c>
+      <c r="C896" s="0" t="s">
+        <v>5235</v>
+      </c>
+      <c r="D896" s="0" t="s">
+        <v>5236</v>
+      </c>
+      <c r="E896" s="0" t="s">
+        <v>5237</v>
+      </c>
+      <c r="F896" s="0" t="s">
+        <v>5238</v>
+      </c>
+      <c r="G896" s="0" t="s">
+        <v>5239</v>
+      </c>
+      <c r="H896" s="0" t="s">
+        <v>609</v>
+      </c>
+      <c r="I896" s="0" t="s">
+        <v>5240</v>
+      </c>
+      <c r="J896" s="0" t="s">
+        <v>5241</v>
+      </c>
+      <c r="K896" s="0" t="s">
+        <v>5147</v>
+      </c>
+    </row>
+    <row r="897" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A897" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B897" s="0" t="s">
+        <v>5242</v>
+      </c>
+      <c r="C897" s="0" t="s">
+        <v>5243</v>
+      </c>
+      <c r="D897" s="0" t="s">
+        <v>5244</v>
+      </c>
+      <c r="E897" s="0" t="s">
+        <v>5245</v>
+      </c>
+      <c r="F897" s="0" t="s">
+        <v>5246</v>
+      </c>
+      <c r="G897" s="0" t="s">
+        <v>5239</v>
+      </c>
+      <c r="H897" s="0" t="s">
+        <v>5247</v>
+      </c>
+      <c r="I897" s="0" t="s">
+        <v>5248</v>
+      </c>
+      <c r="J897" s="0" t="s">
+        <v>5249</v>
+      </c>
+      <c r="K897" s="0" t="s">
+        <v>5151</v>
+      </c>
+    </row>
+    <row r="898" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A898" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B898" s="0" t="s">
+        <v>5250</v>
+      </c>
+      <c r="C898" s="0" t="s">
+        <v>660</v>
+      </c>
+      <c r="D898" s="0" t="s">
+        <v>5251</v>
+      </c>
+      <c r="E898" s="0" t="s">
+        <v>662</v>
+      </c>
+      <c r="F898" s="0" t="s">
+        <v>663</v>
+      </c>
+      <c r="G898" s="0" t="s">
+        <v>5239</v>
+      </c>
+      <c r="H898" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="I898" s="0" t="s">
+        <v>5252</v>
+      </c>
+      <c r="J898" s="0" t="s">
+        <v>5253</v>
+      </c>
+      <c r="K898" s="0" t="s">
+        <v>5147</v>
+      </c>
+    </row>
+    <row r="899" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A899" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B899" s="0" t="s">
+        <v>5254</v>
+      </c>
+      <c r="C899" s="0" t="s">
+        <v>754</v>
+      </c>
+      <c r="D899" s="0" t="s">
+        <v>755</v>
+      </c>
+      <c r="E899" s="0" t="s">
+        <v>5255</v>
+      </c>
+      <c r="F899" s="0" t="s">
+        <v>5256</v>
+      </c>
+      <c r="G899" s="0" t="s">
+        <v>5257</v>
+      </c>
+      <c r="H899" s="0" t="s">
+        <v>911</v>
+      </c>
+      <c r="I899" s="0" t="s">
+        <v>5171</v>
+      </c>
+      <c r="J899" s="0" t="s">
+        <v>5172</v>
+      </c>
+      <c r="K899" s="0" t="s">
+        <v>5151</v>
+      </c>
+    </row>
+    <row r="900" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A900" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B900" s="0" t="s">
+        <v>5258</v>
+      </c>
+      <c r="C900" s="0" t="s">
+        <v>5258</v>
+      </c>
+      <c r="D900" s="0" t="s">
+        <v>5259</v>
+      </c>
+      <c r="E900" s="0" t="s">
+        <v>5260</v>
+      </c>
+      <c r="F900" s="0" t="s">
+        <v>1173</v>
+      </c>
+      <c r="G900" s="0" t="s">
+        <v>5261</v>
+      </c>
+      <c r="H900" s="0" t="s">
+        <v>3389</v>
+      </c>
+      <c r="I900" s="0" t="s">
+        <v>5262</v>
+      </c>
+      <c r="J900" s="0" t="s">
+        <v>5263</v>
+      </c>
+      <c r="K900" s="0" t="s">
+        <v>5151</v>
+      </c>
+    </row>
+    <row r="901" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A901" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B901" s="0" t="s">
+        <v>5264</v>
+      </c>
+      <c r="C901" s="0" t="s">
+        <v>5264</v>
+      </c>
+      <c r="D901" s="0" t="s">
+        <v>5265</v>
+      </c>
+      <c r="E901" s="0" t="s">
+        <v>2088</v>
+      </c>
+      <c r="F901" s="0" t="s">
+        <v>2095</v>
+      </c>
+      <c r="G901" s="0" t="s">
+        <v>5266</v>
+      </c>
+      <c r="H901" s="0" t="s">
+        <v>803</v>
+      </c>
+      <c r="I901" s="0" t="s">
+        <v>5267</v>
+      </c>
+      <c r="J901" s="0" t="s">
+        <v>5268</v>
+      </c>
+      <c r="K901" s="0" t="s">
+        <v>5147</v>
+      </c>
+    </row>
+    <row r="902" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A902" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B902" s="0" t="s">
+        <v>5269</v>
+      </c>
+      <c r="C902" s="0" t="s">
+        <v>5270</v>
+      </c>
+      <c r="D902" s="0" t="s">
+        <v>5271</v>
+      </c>
+      <c r="E902" s="1" t="s">
+        <v>5272</v>
+      </c>
+      <c r="F902" s="0" t="s">
+        <v>5273</v>
+      </c>
+      <c r="G902" s="0" t="s">
+        <v>5239</v>
+      </c>
+      <c r="H902" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="I902" s="0" t="s">
+        <v>5274</v>
+      </c>
+      <c r="J902" s="0" t="s">
+        <v>5275</v>
+      </c>
+      <c r="K902" s="0" t="s">
+        <v>5147</v>
+      </c>
+      <c r="L902" s="0" t="s">
+        <v>5276</v>
+      </c>
+    </row>
+    <row r="903" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A903" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B903" s="0" t="s">
+        <v>5277</v>
+      </c>
+      <c r="C903" s="0" t="s">
+        <v>5277</v>
+      </c>
+      <c r="D903" s="0" t="s">
+        <v>5278</v>
+      </c>
+      <c r="E903" s="1" t="s">
+        <v>5279</v>
+      </c>
+      <c r="F903" s="0" t="s">
+        <v>755</v>
+      </c>
+      <c r="G903" s="0" t="s">
+        <v>5266</v>
+      </c>
+      <c r="H903" s="0" t="s">
+        <v>5280</v>
+      </c>
+      <c r="I903" s="0" t="s">
+        <v>5171</v>
+      </c>
+      <c r="J903" s="0" t="s">
+        <v>5172</v>
+      </c>
+      <c r="K903" s="0" t="s">
+        <v>5151</v>
+      </c>
+    </row>
+    <row r="904" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A904" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B904" s="0" t="s">
+        <v>5281</v>
+      </c>
+      <c r="C904" s="0" t="s">
+        <v>5282</v>
+      </c>
+      <c r="D904" s="0" t="s">
+        <v>5271</v>
+      </c>
+      <c r="E904" s="0" t="s">
+        <v>5283</v>
+      </c>
+      <c r="F904" s="0" t="s">
+        <v>5284</v>
+      </c>
+      <c r="G904" s="0" t="s">
+        <v>5239</v>
+      </c>
+      <c r="H904" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="I904" s="0" t="s">
+        <v>5285</v>
+      </c>
+      <c r="J904" s="0" t="s">
+        <v>5286</v>
+      </c>
+      <c r="K904" s="0" t="s">
+        <v>5147</v>
+      </c>
+    </row>
+    <row r="905" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A905" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B905" s="0" t="s">
+        <v>5287</v>
+      </c>
+      <c r="C905" s="0" t="s">
+        <v>5287</v>
+      </c>
+      <c r="D905" s="0" t="s">
+        <v>5288</v>
+      </c>
+      <c r="E905" s="0" t="s">
+        <v>3312</v>
+      </c>
+      <c r="F905" s="0" t="s">
+        <v>3313</v>
+      </c>
+      <c r="G905" s="0" t="s">
+        <v>5289</v>
+      </c>
+      <c r="H905" s="0" t="s">
+        <v>5290</v>
+      </c>
+      <c r="I905" s="0" t="s">
+        <v>5291</v>
+      </c>
+      <c r="J905" s="0" t="s">
+        <v>5292</v>
+      </c>
+      <c r="K905" s="0" t="s">
+        <v>5083</v>
+      </c>
+    </row>
+    <row r="906" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A906" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B906" s="0" t="s">
+        <v>5293</v>
+      </c>
+      <c r="C906" s="0" t="s">
+        <v>5294</v>
+      </c>
+      <c r="D906" s="0" t="s">
+        <v>5295</v>
+      </c>
+      <c r="E906" s="0" t="s">
+        <v>5296</v>
+      </c>
+      <c r="F906" s="0" t="s">
+        <v>5238</v>
+      </c>
+      <c r="G906" s="0" t="s">
+        <v>5239</v>
+      </c>
+      <c r="H906" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="I906" s="0" t="s">
+        <v>5297</v>
+      </c>
+      <c r="J906" s="0" t="s">
+        <v>5298</v>
+      </c>
+      <c r="K906" s="0" t="s">
+        <v>5147</v>
+      </c>
+    </row>
+    <row r="907" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A907" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B907" s="0" t="s">
+        <v>5299</v>
+      </c>
+      <c r="C907" s="0" t="s">
+        <v>5299</v>
+      </c>
+      <c r="D907" s="0" t="s">
+        <v>5300</v>
+      </c>
+      <c r="E907" s="0" t="s">
+        <v>5301</v>
+      </c>
+      <c r="F907" s="0" t="s">
+        <v>5302</v>
+      </c>
+      <c r="G907" s="0" t="s">
+        <v>5266</v>
+      </c>
+      <c r="I907" s="0" t="s">
+        <v>5303</v>
+      </c>
+      <c r="J907" s="0" t="s">
+        <v>5304</v>
+      </c>
+      <c r="K907" s="0" t="s">
+        <v>5305</v>
+      </c>
+    </row>
+    <row r="908" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A908" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B908" s="0" t="s">
+        <v>5306</v>
+      </c>
+      <c r="C908" s="0" t="s">
+        <v>5306</v>
+      </c>
+      <c r="D908" s="0" t="s">
+        <v>5307</v>
+      </c>
+      <c r="E908" s="0" t="s">
+        <v>5308</v>
+      </c>
+      <c r="F908" s="0" t="s">
+        <v>5309</v>
+      </c>
+      <c r="G908" s="0" t="s">
+        <v>5239</v>
+      </c>
+      <c r="H908" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="I908" s="0" t="s">
+        <v>5310</v>
+      </c>
+      <c r="J908" s="0" t="s">
+        <v>5311</v>
+      </c>
+      <c r="K908" s="0" t="s">
+        <v>5151</v>
+      </c>
+    </row>
+    <row r="909" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A909" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B909" s="0" t="s">
+        <v>5312</v>
+      </c>
+      <c r="C909" s="0" t="s">
+        <v>5313</v>
+      </c>
+      <c r="D909" s="0" t="s">
+        <v>5314</v>
+      </c>
+      <c r="E909" s="0" t="s">
+        <v>5315</v>
+      </c>
+      <c r="F909" s="0" t="s">
+        <v>5316</v>
+      </c>
+      <c r="G909" s="0" t="s">
+        <v>5317</v>
+      </c>
+      <c r="H909" s="0" t="s">
+        <v>5318</v>
+      </c>
+      <c r="I909" s="0" t="s">
+        <v>5319</v>
+      </c>
+      <c r="J909" s="0" t="s">
+        <v>5320</v>
+      </c>
+      <c r="K909" s="0" t="s">
+        <v>5151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>